<commit_message>
Updated Master Trans file.
</commit_message>
<xml_diff>
--- a/Trans Files/Master_Translation_All_Languages.xlsx
+++ b/Trans Files/Master_Translation_All_Languages.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="60" windowWidth="18120" windowHeight="8700"/>
@@ -10,14 +10,14 @@
     <sheet name="UI_Strings" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">UI_Strings!$A$1:$H$115</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">UI_Strings!$A$1:$H$117</definedName>
   </definedNames>
   <calcPr calcId="125725" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="425">
   <si>
     <t>Source (English)</t>
   </si>
@@ -1162,6 +1162,330 @@
   <si>
     <t>Search bar scope button titles
 The publication is active</t>
+  </si>
+  <si>
+    <t>%@ km entfernt</t>
+  </si>
+  <si>
+    <t>über uns</t>
+  </si>
+  <si>
+    <t>aktiv</t>
+  </si>
+  <si>
+    <t>aktiv bis %@</t>
+  </si>
+  <si>
+    <t>Aktivitäten</t>
+  </si>
+  <si>
+    <t>Bild hinzufügen</t>
+  </si>
+  <si>
+    <t>weitere Details</t>
+  </si>
+  <si>
+    <t>Bitte alle Felder ausfüllen</t>
+  </si>
+  <si>
+    <t>ein Fehler ist aufgetreten</t>
+  </si>
+  <si>
+    <t>Jemand anders ist ebenfalls auf dem Weg, es abzuholen</t>
+  </si>
+  <si>
+    <t>Bist Du sicher?</t>
+  </si>
+  <si>
+    <t>zurück</t>
+  </si>
+  <si>
+    <t>anrufen</t>
+  </si>
+  <si>
+    <t>Abholer anrufen</t>
+  </si>
+  <si>
+    <t>Anbieter anrufen</t>
+  </si>
+  <si>
+    <t>Kamera</t>
+  </si>
+  <si>
+    <t>Abbruch</t>
+  </si>
+  <si>
+    <t>am Nächsten</t>
+  </si>
+  <si>
+    <t>Kommunikations-Probleme (Verbindung etc.)</t>
+  </si>
+  <si>
+    <t>Bestätige, dass die Gelegenheit beendet ist</t>
+  </si>
+  <si>
+    <t>sehr gut!</t>
+  </si>
+  <si>
+    <t>aktueller Standort</t>
+  </si>
+  <si>
+    <t>löschen</t>
+  </si>
+  <si>
+    <t>Gelegenheit löschen?</t>
+  </si>
+  <si>
+    <t>Beschreibung</t>
+  </si>
+  <si>
+    <t>fertig</t>
+  </si>
+  <si>
+    <t>bearbeiten</t>
+  </si>
+  <si>
+    <t>unterwegs</t>
+  </si>
+  <si>
+    <t>beendet</t>
+  </si>
+  <si>
+    <t>endet</t>
+  </si>
+  <si>
+    <t>endet:</t>
+  </si>
+  <si>
+    <t>Eine Gelegenheit in Deiner Nähe ist zu Ende</t>
+  </si>
+  <si>
+    <t>Ort der Gelegenheit</t>
+  </si>
+  <si>
+    <t>Gelegenheiten in Deiner Nähe</t>
+  </si>
+  <si>
+    <t>Hallo. Was möchtest Du anbieten</t>
+  </si>
+  <si>
+    <t>Ich möchte %@ mitnehmen</t>
+  </si>
+  <si>
+    <t>inaktiv</t>
+  </si>
+  <si>
+    <t>inkorrekte Telefonnummer</t>
+  </si>
+  <si>
+    <t>Die Telefonnummer scheint nicht zu stimmen. Bitte überprüfe sie.</t>
+  </si>
+  <si>
+    <t>letzte Suchanfragen</t>
+  </si>
+  <si>
+    <t>Galerie</t>
+  </si>
+  <si>
+    <t>Nachricht konnte nicht gesendet werden</t>
+  </si>
+  <si>
+    <t>meine Abholungen</t>
+  </si>
+  <si>
+    <t>meine Angebote</t>
+  </si>
+  <si>
+    <t>Navigieren mit:</t>
+  </si>
+  <si>
+    <t>neue Mitnahmegelegenheit</t>
+  </si>
+  <si>
+    <t>neue Mitnahmegelegenheit in Deiner Nähe</t>
+  </si>
+  <si>
+    <t>Eine neue Gelegenheit wurde aktualisiert</t>
+  </si>
+  <si>
+    <t>nein</t>
+  </si>
+  <si>
+    <t>Keine Mitnehmer wurden ausgewählt.</t>
+  </si>
+  <si>
+    <t>kein Name</t>
+  </si>
+  <si>
+    <t>Es ist noch niemand zur Mitnahme eingetragen</t>
+  </si>
+  <si>
+    <t>keine Telefonnummer</t>
+  </si>
+  <si>
+    <t>keine Berichte</t>
+  </si>
+  <si>
+    <t>nicht jetzt</t>
+  </si>
+  <si>
+    <t>nichts übrig</t>
+  </si>
+  <si>
+    <t>nicht veröffentlicht</t>
+  </si>
+  <si>
+    <t>veröffentlicht</t>
+  </si>
+  <si>
+    <t>Optionen</t>
+  </si>
+  <si>
+    <t>Telefonnummer</t>
+  </si>
+  <si>
+    <t>mitnehmen</t>
+  </si>
+  <si>
+    <t>Mitnahme endet:</t>
+  </si>
+  <si>
+    <t>Essen mitnehmen</t>
+  </si>
+  <si>
+    <t>Mitnahme beginnt:</t>
+  </si>
+  <si>
+    <t>Bitte ausfüllen um mitzumachen:</t>
+  </si>
+  <si>
+    <t>Bitte nur berichten, wenn Du vor Ort warst.</t>
+  </si>
+  <si>
+    <t>vorherige Suchanfragen</t>
+  </si>
+  <si>
+    <t>zuletzt</t>
+  </si>
+  <si>
+    <t>hierfür anmelden</t>
+  </si>
+  <si>
+    <t>mich für die Mitnahme anmelden</t>
+  </si>
+  <si>
+    <t>Gelegenheit entfernen</t>
+  </si>
+  <si>
+    <t>Bericht</t>
+  </si>
+  <si>
+    <t>Berichte</t>
+  </si>
+  <si>
+    <t>suchen</t>
+  </si>
+  <si>
+    <t>Adresse auswählen</t>
+  </si>
+  <si>
+    <t>alles auswählen</t>
+  </si>
+  <si>
+    <t>gewähltes Bild</t>
+  </si>
+  <si>
+    <t>Nachricht senden</t>
+  </si>
+  <si>
+    <t>Anbieten</t>
+  </si>
+  <si>
+    <t>Essen anbieten</t>
+  </si>
+  <si>
+    <t>Details anzeigen</t>
+  </si>
+  <si>
+    <t>Gelegenheit zeigen</t>
+  </si>
+  <si>
+    <t>begonnen:</t>
+  </si>
+  <si>
+    <t>Gelegenheit beenden</t>
+  </si>
+  <si>
+    <t>Es gibt keine gültigen Telefonnummern</t>
+  </si>
+  <si>
+    <t>Es gibt mehr mitzunehmen</t>
+  </si>
+  <si>
+    <t>alles mitgenommen</t>
+  </si>
+  <si>
+    <t>nochmal versuchen</t>
+  </si>
+  <si>
+    <t>nochmal versuchen?</t>
+  </si>
+  <si>
+    <t>Gibt die Adresse ein oder wähle eine frühere Mitnahme aus</t>
+  </si>
+  <si>
+    <t>Benutzer</t>
+  </si>
+  <si>
+    <t>Nutzerberichte</t>
+  </si>
+  <si>
+    <t>Nutzer die zum Abholen vorbeikommen</t>
+  </si>
+  <si>
+    <t>Willkommen</t>
+  </si>
+  <si>
+    <t>Was bietest Du an?</t>
+  </si>
+  <si>
+    <t>Was möchtest Du tun?</t>
+  </si>
+  <si>
+    <t>Was ist Deine Telefonnummer?</t>
+  </si>
+  <si>
+    <t>Ja</t>
+  </si>
+  <si>
+    <t>Du bist weit von dem Ort der Gelegenheit entgernt.</t>
+  </si>
+  <si>
+    <t>Du bist bei %@ angekommen.</t>
+  </si>
+  <si>
+    <t>Feedback senden</t>
+  </si>
+  <si>
+    <t>Teile Deine Gedanken oder irgendetwas mit</t>
+  </si>
+  <si>
+    <t>absenden</t>
+  </si>
+  <si>
+    <t>Collect</t>
+  </si>
+  <si>
+    <t>Address Selector</t>
+  </si>
+  <si>
+    <t>בחר כתובת</t>
+  </si>
+  <si>
+    <t>Class = "UIViewController"; title = "Address Selector"; ObjectID = "hdu-mN-4y2";</t>
+  </si>
+  <si>
+    <t>Class = "UIViewController"; title = "Collect"; ObjectID = "vXZ-lx-hvc";</t>
   </si>
 </sst>
 </file>
@@ -1200,7 +1524,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1210,6 +1534,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1226,7 +1556,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
@@ -1240,26 +1570,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" readingOrder="2"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -1548,24 +1888,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H115"/>
+  <dimension ref="A1:H117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="35.25" style="4" customWidth="1"/>
+    <col min="1" max="1" width="28.75" style="8" customWidth="1"/>
     <col min="2" max="2" width="55.75" style="4" customWidth="1"/>
     <col min="3" max="3" width="41.75" style="4" customWidth="1"/>
-    <col min="4" max="5" width="9.875" style="7" customWidth="1"/>
-    <col min="6" max="6" width="42.875" style="4" customWidth="1"/>
-    <col min="7" max="16384" width="9" style="4"/>
+    <col min="4" max="5" width="9.875" style="6" customWidth="1"/>
+    <col min="6" max="6" width="31.625" style="8" customWidth="1"/>
+    <col min="7" max="7" width="31.625" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
@@ -1574,13 +1915,13 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
@@ -1597,11 +1938,14 @@
       <c r="B2" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F2" s="5" t="s">
+      <c r="D2" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F2" s="9" t="s">
         <v>203</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="28.5">
@@ -1611,11 +1955,14 @@
       <c r="B3" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F3" s="5" t="s">
+      <c r="D3" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F3" s="9" t="s">
         <v>204</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="28.5">
@@ -1625,11 +1972,14 @@
       <c r="B4" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F4" s="5" t="s">
+      <c r="D4" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>205</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="42.75">
@@ -1639,11 +1989,14 @@
       <c r="B5" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="9" t="s">
         <v>314</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1653,11 +2006,14 @@
       <c r="B6" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F6" s="5" t="s">
+      <c r="D6" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F6" s="9" t="s">
         <v>206</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -1667,11 +2023,14 @@
       <c r="B7" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F7" s="5" t="s">
+      <c r="D7" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F7" s="9" t="s">
         <v>207</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -1681,1500 +2040,1858 @@
       <c r="B8" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F8" s="5" t="s">
+      <c r="D8" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F8" s="9" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="G8" s="8" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="28.5">
       <c r="A9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>209</v>
-      </c>
+        <v>421</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>423</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>422</v>
+      </c>
+      <c r="G9" s="12"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>210</v>
+        <v>126</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="28.5">
+      <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F11" s="5" t="s">
+      <c r="D12" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F12" s="9" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>212</v>
+      <c r="G12" s="8" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="2" t="s">
-        <v>18</v>
+        <v>212</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>215</v>
+        <v>126</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>216</v>
+        <v>128</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="D16" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F16" s="5" t="s">
+      <c r="D17" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F17" s="9" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="2" t="s">
+      <c r="G17" s="8" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D17" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F17" s="5" t="s">
+      <c r="D18" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F18" s="9" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="2" t="s">
+      <c r="G18" s="8" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="D18" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F18" s="5" t="s">
+      <c r="D19" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F19" s="9" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="2" t="s">
+      <c r="G19" s="8" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B20" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D19" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F19" s="5" t="s">
+      <c r="D20" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F20" s="9" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="2" t="s">
+      <c r="G20" s="8" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B21" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D20" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F20" s="5" t="s">
+      <c r="D21" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F21" s="9" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="2" t="s">
+      <c r="G21" s="8" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="28.5">
+      <c r="A22" s="10" t="s">
+        <v>420</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>424</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="G22" s="12"/>
+    </row>
+    <row r="23" spans="1:7" ht="28.5">
+      <c r="A23" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B23" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="D21" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F21" s="5" t="s">
+      <c r="D23" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F23" s="9" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="2" t="s">
+      <c r="G23" s="8" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="28.5">
+      <c r="A24" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B24" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="D22" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F22" s="5" t="s">
+      <c r="D24" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F24" s="9" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="2" t="s">
+      <c r="G24" s="8" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B25" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="D23" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F23" s="5" t="s">
+      <c r="D25" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F25" s="9" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="2" t="s">
+      <c r="G25" s="8" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B26" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="D24" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F24" s="5" t="s">
+      <c r="D26" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F26" s="9" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="2" t="s">
+      <c r="G26" s="8" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="D25" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F25" s="5" t="s">
+      <c r="D27" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F27" s="9" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="2" t="s">
+      <c r="G27" s="8" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B28" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="D26" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F26" s="5" t="s">
+      <c r="D28" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F28" s="9" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="2" t="s">
+      <c r="G28" s="8" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B29" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="D27" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F27" s="5" t="s">
+      <c r="D29" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F29" s="9" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="2" t="s">
+      <c r="G29" s="8" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B30" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="D28" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F28" s="5" t="s">
+      <c r="D30" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F30" s="9" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="2" t="s">
+      <c r="G30" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B31" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D29" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F29" s="5" t="s">
+      <c r="D31" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F31" s="9" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="2" t="s">
+      <c r="G31" s="8" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B32" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="D30" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F30" s="5" t="s">
+      <c r="D32" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F32" s="9" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" ht="42.75">
-      <c r="A31" s="2" t="s">
+      <c r="G32" s="8" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="42.75">
+      <c r="A33" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B33" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="D31" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F31" s="5" t="s">
+      <c r="D33" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F33" s="9" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="2" t="s">
+      <c r="G33" s="8" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B34" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="D32" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F32" s="5" t="s">
+      <c r="D34" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F34" s="9" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="2" t="s">
+      <c r="G34" s="8" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B35" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D33" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F33" s="5" t="s">
+      <c r="D35" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F35" s="9" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="2" t="s">
+      <c r="G35" s="8" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B36" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="D34" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F34" s="5" t="s">
+      <c r="D36" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F36" s="9" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" ht="28.5">
-      <c r="A35" s="2" t="s">
+      <c r="G36" s="8" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="28.5">
+      <c r="A37" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B37" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="D35" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F35" s="5" t="s">
+      <c r="D37" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F37" s="9" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" s="2" t="s">
+      <c r="G37" s="12"/>
+    </row>
+    <row r="38" spans="1:7" ht="28.5">
+      <c r="A38" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B38" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="D36" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F36" s="5" t="s">
+      <c r="D38" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F38" s="9" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="2" t="s">
+      <c r="G38" s="8" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B39" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="D37" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F37" s="5" t="s">
+      <c r="D39" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F39" s="9" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38" s="2" t="s">
+      <c r="G39" s="8" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="28.5">
+      <c r="A40" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B40" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="D38" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F38" s="5" t="s">
+      <c r="D40" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F40" s="9" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="2" t="s">
+      <c r="G40" s="8" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B41" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="F39" s="5" t="s">
+      <c r="D41" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F41" s="9" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" s="2" t="s">
+      <c r="G41" s="8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="28.5">
+      <c r="A42" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B42" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="D40" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F40" s="5" t="s">
+      <c r="D42" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F42" s="9" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" ht="42.75">
-      <c r="A41" s="2" t="s">
+      <c r="G42" s="8" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="42.75">
+      <c r="A43" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B43" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="D41" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F41" s="5" t="s">
+      <c r="D43" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F43" s="9" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="A42" s="2" t="s">
+      <c r="G43" s="8" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B44" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="D42" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F42" s="5" t="s">
+      <c r="D44" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F44" s="9" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="43" spans="1:6">
-      <c r="A43" s="2" t="s">
+      <c r="G44" s="8" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B45" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="D43" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F43" s="5" t="s">
+      <c r="D45" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F45" s="9" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" ht="28.5">
-      <c r="A44" s="2" t="s">
+      <c r="G45" s="8" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="42.75">
+      <c r="A46" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B46" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D44" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F44" s="5" t="s">
+      <c r="D46" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F46" s="9" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="45" spans="1:6">
-      <c r="A45" s="2" t="s">
+      <c r="G46" s="8" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B47" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="D45" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F45" s="5" t="s">
+      <c r="D47" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F47" s="9" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="46" spans="1:6">
-      <c r="A46" s="2" t="s">
+      <c r="G47" s="8" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B48" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="D46" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F46" s="5" t="s">
+      <c r="D48" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F48" s="9" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="47" spans="1:6">
-      <c r="A47" s="2" t="s">
+      <c r="G48" s="8" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="28.5">
+      <c r="A49" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B49" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="D47" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F47" s="5" t="s">
+      <c r="D49" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F49" s="9" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" ht="28.5">
-      <c r="A48" s="2" t="s">
+      <c r="G49" s="8" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="28.5">
+      <c r="A50" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B50" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="D48" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F48" s="5" t="s">
+      <c r="D50" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F50" s="9" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" ht="28.5">
-      <c r="A49" s="2" t="s">
+      <c r="G50" s="8" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="28.5">
+      <c r="A51" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B51" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="D49" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F49" s="5" t="s">
+      <c r="D51" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F51" s="9" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="50" spans="1:6">
-      <c r="A50" s="2" t="s">
+      <c r="G51" s="8" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B52" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="D50" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F50" s="5" t="s">
+      <c r="D52" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F52" s="9" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="51" spans="1:6">
-      <c r="A51" s="2" t="s">
+      <c r="G52" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B53" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="D51" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F51" s="5" t="s">
+      <c r="D53" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F53" s="9" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="52" spans="1:6">
-      <c r="A52" s="2" t="s">
+      <c r="G53" s="8" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B54" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="D52" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F52" s="5" t="s">
+      <c r="D54" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F54" s="9" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" ht="28.5">
-      <c r="A53" s="2" t="s">
+      <c r="G54" s="8" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="28.5">
+      <c r="A55" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B55" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="D53" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F53" s="5" t="s">
+      <c r="D55" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F55" s="9" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="54" spans="1:6">
-      <c r="A54" s="2" t="s">
+      <c r="G55" s="8" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="28.5">
+      <c r="A56" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B56" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="D54" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F54" s="5" t="s">
+      <c r="D56" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F56" s="9" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="55" spans="1:6">
-      <c r="A55" s="2" t="s">
+      <c r="G56" s="8" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B57" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D55" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F55" s="5" t="s">
+      <c r="D57" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F57" s="9" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="56" spans="1:6">
-      <c r="A56" s="2" t="s">
+      <c r="G57" s="8" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="28.5">
+      <c r="A58" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B58" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="D56" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F56" s="5" t="s">
+      <c r="D58" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F58" s="9" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="57" spans="1:6">
-      <c r="A57" s="2" t="s">
+      <c r="G58" s="8" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B59" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="D57" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F57" s="5" t="s">
+      <c r="D59" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F59" s="9" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="58" spans="1:6">
-      <c r="A58" s="2" t="s">
+      <c r="G59" s="8" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="28.5">
+      <c r="A60" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B58" s="2"/>
-      <c r="D58" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F58" s="5" t="s">
+      <c r="B60" s="2"/>
+      <c r="D60" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F60" s="9" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" ht="28.5">
-      <c r="A59" s="2" t="s">
+      <c r="G60" s="8" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="28.5">
+      <c r="A61" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="B61" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="D59" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F59" s="5" t="s">
+      <c r="D61" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F61" s="9" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" ht="28.5">
-      <c r="A60" s="2" t="s">
+      <c r="G61" s="8" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="28.5">
+      <c r="A62" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B62" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="D60" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F60" s="5" t="s">
+      <c r="D62" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F62" s="9" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="61" spans="1:6">
-      <c r="A61" s="2" t="s">
+      <c r="G62" s="8" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B63" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="D61" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F61" s="5" t="s">
+      <c r="D63" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F63" s="9" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" ht="28.5">
-      <c r="A62" s="2" t="s">
+      <c r="G63" s="8" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="28.5">
+      <c r="A64" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B64" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="D62" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F62" s="5" t="s">
+      <c r="D64" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F64" s="9" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="63" spans="1:6">
-      <c r="A63" s="2" t="s">
+      <c r="G64" s="8" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
+      <c r="A65" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B65" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="D63" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F63" s="5" t="s">
+      <c r="D65" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F65" s="9" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="64" spans="1:6">
-      <c r="A64" s="2" t="s">
+      <c r="G65" s="8" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="A66" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="D64" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F64" s="5" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6">
-      <c r="A65" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="D65" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F65" s="5" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6">
-      <c r="A66" s="2" t="s">
-        <v>69</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D66" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F66" s="5" t="s">
+      <c r="D66" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F66" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="G66" s="8" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
+      <c r="A67" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F67" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="G67" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="A68" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D68" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F68" s="9" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="67" spans="1:6">
-      <c r="A67" s="2" t="s">
+      <c r="G68" s="8" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="A69" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B69" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="D67" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F67" s="5" t="s">
+      <c r="D69" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F69" s="9" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="68" spans="1:6">
-      <c r="A68" s="2" t="s">
+      <c r="G69" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
+      <c r="A70" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B70" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="D68" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F68" s="5" t="s">
+      <c r="D70" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F70" s="9" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="69" spans="1:6">
-      <c r="A69" s="2" t="s">
+      <c r="G70" s="8" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
+      <c r="A71" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B71" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="D69" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F69" s="5" t="s">
+      <c r="D71" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F71" s="9" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="70" spans="1:6">
-      <c r="A70" s="2" t="s">
+      <c r="G71" s="8" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="A72" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B72" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="D70" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F70" s="5" t="s">
+      <c r="D72" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F72" s="9" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="71" spans="1:6">
-      <c r="A71" s="2" t="s">
+      <c r="G72" s="8" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
+      <c r="A73" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="B73" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="D71" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F71" s="5" t="s">
+      <c r="D73" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F73" s="9" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" ht="28.5">
-      <c r="A72" s="2" t="s">
+      <c r="G73" s="8" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="28.5">
+      <c r="A74" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="B74" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="D72" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F72" s="5" t="s">
+      <c r="D74" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F74" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="73" spans="1:6">
-      <c r="A73" s="2" t="s">
+      <c r="G74" s="8" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
+      <c r="A75" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="B75" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="D73" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F73" s="5" t="s">
+      <c r="D75" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F75" s="9" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="74" spans="1:6">
-      <c r="A74" s="2" t="s">
+      <c r="G75" s="8" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="28.5">
+      <c r="A76" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B74" s="2" t="s">
+      <c r="B76" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D74" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F74" s="5" t="s">
+      <c r="D76" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F76" s="9" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" ht="28.5">
-      <c r="A75" s="2" t="s">
+      <c r="G76" s="8" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="28.5">
+      <c r="A77" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B75" s="2"/>
-      <c r="D75" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F75" s="5" t="s">
+      <c r="B77" s="2"/>
+      <c r="D77" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F77" s="9" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" ht="28.5">
-      <c r="A76" s="2" t="s">
+      <c r="G77" s="8" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="28.5">
+      <c r="A78" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="B78" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="D76" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F76" s="5" t="s">
+      <c r="D78" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F78" s="9" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="77" spans="1:6">
-      <c r="A77" s="2" t="s">
+      <c r="G78" s="8" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
+      <c r="A79" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="B79" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D77" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F77" s="5" t="s">
+      <c r="D79" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F79" s="9" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="78" spans="1:6">
-      <c r="A78" s="2" t="s">
+      <c r="G79" s="8" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
+      <c r="A80" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="B80" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="D78" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F78" s="5" t="s">
+      <c r="D80" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F80" s="9" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="79" spans="1:6">
-      <c r="A79" s="2" t="s">
+      <c r="G80" s="8" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="28.5">
+      <c r="A81" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="B81" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="D79" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F79" s="5" t="s">
+      <c r="D81" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F81" s="9" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="80" spans="1:6">
-      <c r="A80" s="2" t="s">
+      <c r="G81" s="8" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
+      <c r="A82" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B80" s="2" t="s">
+      <c r="B82" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="D80" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F80" s="5" t="s">
+      <c r="D82" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F82" s="9" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="81" spans="1:6">
-      <c r="A81" s="2" t="s">
+      <c r="G82" s="8" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
+      <c r="A83" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="B83" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="D81" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F81" s="5" t="s">
+      <c r="D83" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F83" s="9" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" ht="28.5">
-      <c r="A82" s="2" t="s">
+      <c r="G83" s="8" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="28.5">
+      <c r="A84" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="B84" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="D82" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F82" s="5" t="s">
+      <c r="D84" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F84" s="9" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="83" spans="1:6">
-      <c r="A83" s="2" t="s">
+      <c r="G84" s="8" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
+      <c r="A85" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="B85" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="D83" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F83" s="5" t="s">
+      <c r="D85" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F85" s="9" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="84" spans="1:6">
-      <c r="A84" s="2" t="s">
+      <c r="G85" s="8" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
+      <c r="A86" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="B86" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="D84" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F84" s="5" t="s">
+      <c r="D86" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F86" s="9" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="85" spans="1:6">
-      <c r="A85" s="2" t="s">
+      <c r="G86" s="8" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
+      <c r="A87" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B85" s="2" t="s">
+      <c r="B87" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="D85" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F85" s="5" t="s">
+      <c r="D87" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F87" s="9" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="86" spans="1:6">
-      <c r="A86" s="2" t="s">
+      <c r="G87" s="8" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
+      <c r="A88" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="B88" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="D86" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F86" s="5" t="s">
+      <c r="D88" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F88" s="9" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" ht="28.5">
-      <c r="A87" s="2" t="s">
+      <c r="G88" s="8" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="28.5">
+      <c r="A89" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B87" s="2" t="s">
+      <c r="B89" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="D87" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F87" s="5" t="s">
+      <c r="D89" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F89" s="9" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="88" spans="1:6">
-      <c r="A88" s="2" t="s">
+      <c r="G89" s="8" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7">
+      <c r="A90" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B88" s="2" t="s">
+      <c r="B90" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="D88" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F88" s="5" t="s">
+      <c r="D90" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F90" s="9" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="89" spans="1:6">
-      <c r="A89" s="2" t="s">
+      <c r="G90" s="8" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7">
+      <c r="A91" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B89" s="2" t="s">
+      <c r="B91" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="D89" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F89" s="5" t="s">
+      <c r="D91" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F91" s="9" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="90" spans="1:6">
-      <c r="A90" s="2" t="s">
+      <c r="G91" s="8" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7">
+      <c r="A92" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B90" s="2" t="s">
+      <c r="B92" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="D90" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F90" s="5" t="s">
+      <c r="D92" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F92" s="9" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" ht="28.5">
-      <c r="A91" s="2" t="s">
+      <c r="G92" s="8" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" ht="28.5">
+      <c r="A93" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B91" s="2" t="s">
+      <c r="B93" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="D91" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F91" s="5" t="s">
+      <c r="D93" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F93" s="9" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="92" spans="1:6">
-      <c r="A92" s="2" t="s">
+      <c r="G93" s="8" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" ht="28.5">
+      <c r="A94" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B92" s="2" t="s">
+      <c r="B94" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="F92" s="5" t="s">
+      <c r="D94" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F94" s="9" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" ht="28.5">
-      <c r="A93" s="2" t="s">
+      <c r="G94" s="8" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" ht="28.5">
+      <c r="A95" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B93" s="2" t="s">
+      <c r="B95" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="D93" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F93" s="5" t="s">
+      <c r="D95" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F95" s="9" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="94" spans="1:6">
-      <c r="A94" s="2" t="s">
+      <c r="G95" s="8" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7">
+      <c r="A96" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B94" s="2" t="s">
+      <c r="B96" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="D94" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F94" s="5" t="s">
+      <c r="D96" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F96" s="9" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="95" spans="1:6">
-      <c r="A95" s="2" t="s">
+      <c r="G96" s="8" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7">
+      <c r="A97" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B95" s="2" t="s">
+      <c r="B97" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="D95" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F95" s="5" t="s">
+      <c r="D97" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F97" s="9" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="96" spans="1:6">
-      <c r="A96" s="2" t="s">
+      <c r="G97" s="8" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7">
+      <c r="A98" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B96" s="2" t="s">
+      <c r="B98" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="D96" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F96" s="5" t="s">
+      <c r="D98" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F98" s="9" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="97" spans="1:6">
-      <c r="A97" s="2" t="s">
+      <c r="G98" s="8" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" ht="28.5">
+      <c r="A99" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B97" s="2"/>
-      <c r="D97" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F97" s="5" t="s">
+      <c r="B99" s="2"/>
+      <c r="D99" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F99" s="9" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" ht="28.5">
-      <c r="A98" s="2" t="s">
+      <c r="G99" s="8" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" ht="28.5">
+      <c r="A100" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B98" s="2" t="s">
+      <c r="B100" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="D98" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F98" s="5" t="s">
+      <c r="D100" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F100" s="9" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" ht="28.5">
-      <c r="A99" s="2" t="s">
+      <c r="G100" s="8" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" ht="28.5">
+      <c r="A101" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B99" s="2" t="s">
+      <c r="B101" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="D99" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F99" s="5" t="s">
+      <c r="D101" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F101" s="9" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" ht="28.5">
-      <c r="A100" s="2" t="s">
+      <c r="G101" s="8" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" ht="28.5">
+      <c r="A102" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B100" s="2" t="s">
+      <c r="B102" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="D100" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F100" s="5" t="s">
+      <c r="D102" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F102" s="9" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="101" spans="1:6">
-      <c r="A101" s="2" t="s">
+      <c r="G102" s="8" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7">
+      <c r="A103" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B101" s="2" t="s">
+      <c r="B103" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="D101" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F101" s="5" t="s">
+      <c r="D103" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F103" s="9" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="102" spans="1:6">
-      <c r="A102" s="2" t="s">
+      <c r="G103" s="8" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7">
+      <c r="A104" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B102" s="2" t="s">
+      <c r="B104" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D102" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F102" s="5" t="s">
+      <c r="D104" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F104" s="9" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="103" spans="1:6">
-      <c r="A103" s="2" t="s">
+      <c r="G104" s="8" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7">
+      <c r="A105" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B103" s="2" t="s">
+      <c r="B105" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D103" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F103" s="5" t="s">
+      <c r="D105" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F105" s="9" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="104" spans="1:6" ht="28.5">
-      <c r="A104" s="2" t="s">
+      <c r="G105" s="8" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" ht="42.75">
+      <c r="A106" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B104" s="2" t="s">
+      <c r="B106" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="D104" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F104" s="5" t="s">
+      <c r="D106" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F106" s="9" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="105" spans="1:6">
-      <c r="A105" s="2" t="s">
+      <c r="G106" s="8" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7">
+      <c r="A107" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B105" s="2"/>
-      <c r="D105" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F105" s="5" t="s">
+      <c r="B107" s="2"/>
+      <c r="D107" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F107" s="9" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="106" spans="1:6">
-      <c r="A106" s="2" t="s">
+      <c r="G107" s="8" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7">
+      <c r="A108" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B106" s="2" t="s">
+      <c r="B108" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="D106" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F106" s="5" t="s">
+      <c r="D108" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F108" s="9" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="107" spans="1:6">
-      <c r="A107" s="2" t="s">
+      <c r="G108" s="8" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" ht="28.5">
+      <c r="A109" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B107" s="2" t="s">
+      <c r="B109" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="D107" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F107" s="5" t="s">
+      <c r="D109" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F109" s="9" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="108" spans="1:6">
-      <c r="A108" s="2" t="s">
+      <c r="G109" s="8" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7">
+      <c r="A110" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="B108" s="2" t="s">
+      <c r="B110" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="D108" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F108" s="5" t="s">
+      <c r="D110" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F110" s="9" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="109" spans="1:6" ht="28.5">
-      <c r="A109" s="2" t="s">
+      <c r="G110" s="8" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" ht="28.5">
+      <c r="A111" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B109" s="2" t="s">
+      <c r="B111" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="D109" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F109" s="5" t="s">
+      <c r="D111" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F111" s="9" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="110" spans="1:6">
-      <c r="A110" s="2" t="s">
+      <c r="G111" s="8" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7">
+      <c r="A112" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B110" s="2" t="s">
+      <c r="B112" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="D110" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F110" s="5" t="s">
+      <c r="D112" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F112" s="9" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="111" spans="1:6" ht="28.5">
-      <c r="A111" s="2" t="s">
+      <c r="G112" s="8" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" ht="28.5">
+      <c r="A113" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B111" s="2" t="s">
+      <c r="B113" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="D111" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F111" s="5" t="s">
+      <c r="D113" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F113" s="9" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="112" spans="1:6">
-      <c r="A112" s="2" t="s">
+      <c r="G113" s="8" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" ht="28.5">
+      <c r="A114" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B112" s="2" t="s">
+      <c r="B114" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="D112" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F112" s="5" t="s">
+      <c r="D114" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F114" s="9" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="113" spans="1:6">
-      <c r="A113" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="B113" s="2" t="s">
+      <c r="G114" s="8" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7">
+      <c r="A115" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B115" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D113" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F113" s="5" t="s">
+      <c r="D115" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F115" s="9" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="114" spans="1:6">
-      <c r="A114" s="2" t="s">
+      <c r="G115" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" ht="28.5">
+      <c r="A116" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="B114" s="2"/>
-      <c r="D114" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F114" s="5" t="s">
+      <c r="B116" s="2"/>
+      <c r="D116" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F116" s="9" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="115" spans="1:6" ht="42.75">
-      <c r="A115" s="2" t="s">
+      <c r="G116" s="8" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" ht="42.75">
+      <c r="A117" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B115" s="2" t="s">
+      <c r="B117" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="D115" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F115" s="5" t="s">
+      <c r="D117" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F117" s="9" t="s">
         <v>313</v>
       </c>
+      <c r="G117" s="8" t="s">
+        <v>416</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H115"/>
+  <autoFilter ref="A1:H117"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Made small fixes to the German translation.
</commit_message>
<xml_diff>
--- a/Trans Files/Master_Translation_All_Languages.xlsx
+++ b/Trans Files/Master_Translation_All_Languages.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="60" windowWidth="18120" windowHeight="8700"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="426">
   <si>
     <t>Source (English)</t>
   </si>
@@ -1212,9 +1212,6 @@
     <t>Kamera</t>
   </si>
   <si>
-    <t>Abbruch</t>
-  </si>
-  <si>
     <t>am Nächsten</t>
   </si>
   <si>
@@ -1227,9 +1224,6 @@
     <t>sehr gut!</t>
   </si>
   <si>
-    <t>aktueller Standort</t>
-  </si>
-  <si>
     <t>löschen</t>
   </si>
   <si>
@@ -1266,9 +1260,6 @@
     <t>Gelegenheiten in Deiner Nähe</t>
   </si>
   <si>
-    <t>Hallo. Was möchtest Du anbieten</t>
-  </si>
-  <si>
     <t>Ich möchte %@ mitnehmen</t>
   </si>
   <si>
@@ -1486,13 +1477,25 @@
   </si>
   <si>
     <t>Class = "UIViewController"; title = "Collect"; ObjectID = "vXZ-lx-hvc";</t>
+  </si>
+  <si>
+    <t>Apple Karten</t>
+  </si>
+  <si>
+    <t>Hallo, Was möchtest Du anbieten</t>
+  </si>
+  <si>
+    <t>Abbrechen</t>
+  </si>
+  <si>
+    <t>Aktueller Ort</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1600,6 +1603,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1678,6 +1686,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1712,6 +1721,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1887,14 +1897,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H117"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28.75" style="8" customWidth="1"/>
     <col min="2" max="2" width="55.75" style="4" customWidth="1"/>
@@ -1905,7 +1915,7 @@
     <col min="8" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15">
+    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1931,7 +1941,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="71.25">
+    <row r="2" spans="1:8" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1948,7 +1958,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="28.5">
+    <row r="3" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -1965,7 +1975,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="28.5">
+    <row r="4" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -1982,7 +1992,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="42.75">
+    <row r="5" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -1999,7 +2009,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
@@ -2016,7 +2026,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
@@ -2033,7 +2043,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -2050,22 +2060,22 @@
         <v>323</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="28.5">
+    <row r="9" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>112</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="G9" s="12"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -2082,7 +2092,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -2099,7 +2109,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="28.5">
+    <row r="12" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -2116,7 +2126,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>212</v>
       </c>
@@ -2133,10 +2143,10 @@
         <v>212</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
@@ -2153,7 +2163,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
@@ -2170,7 +2180,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
@@ -2187,7 +2197,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
@@ -2204,7 +2214,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
@@ -2221,7 +2231,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>23</v>
       </c>
@@ -2238,7 +2248,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>24</v>
       </c>
@@ -2252,10 +2262,10 @@
         <v>220</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>25</v>
       </c>
@@ -2269,15 +2279,15 @@
         <v>221</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="28.5">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>112</v>
@@ -2287,7 +2297,7 @@
       </c>
       <c r="G22" s="12"/>
     </row>
-    <row r="23" spans="1:7" ht="28.5">
+    <row r="23" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>26</v>
       </c>
@@ -2301,10 +2311,10 @@
         <v>222</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="28.5">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>27</v>
       </c>
@@ -2318,10 +2328,10 @@
         <v>223</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>28</v>
       </c>
@@ -2335,10 +2345,10 @@
         <v>224</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>29</v>
       </c>
@@ -2352,10 +2362,10 @@
         <v>225</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>30</v>
       </c>
@@ -2369,10 +2379,10 @@
         <v>226</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>31</v>
       </c>
@@ -2386,10 +2396,10 @@
         <v>227</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>32</v>
       </c>
@@ -2403,10 +2413,10 @@
         <v>228</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>33</v>
       </c>
@@ -2423,7 +2433,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>34</v>
       </c>
@@ -2437,10 +2447,10 @@
         <v>230</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>35</v>
       </c>
@@ -2454,10 +2464,10 @@
         <v>231</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="42.75">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>36</v>
       </c>
@@ -2471,10 +2481,10 @@
         <v>232</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>37</v>
       </c>
@@ -2488,10 +2498,10 @@
         <v>233</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>38</v>
       </c>
@@ -2505,10 +2515,10 @@
         <v>234</v>
       </c>
       <c r="G35" s="8" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>39</v>
       </c>
@@ -2522,10 +2532,10 @@
         <v>235</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="28.5">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>236</v>
       </c>
@@ -2540,7 +2550,7 @@
       </c>
       <c r="G37" s="12"/>
     </row>
-    <row r="38" spans="1:7" ht="28.5">
+    <row r="38" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>40</v>
       </c>
@@ -2554,10 +2564,10 @@
         <v>238</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>41</v>
       </c>
@@ -2571,10 +2581,10 @@
         <v>239</v>
       </c>
       <c r="G39" s="8" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="28.5">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>42</v>
       </c>
@@ -2588,10 +2598,10 @@
         <v>240</v>
       </c>
       <c r="G40" s="8" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>117</v>
       </c>
@@ -2608,7 +2618,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="28.5">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>43</v>
       </c>
@@ -2622,10 +2632,10 @@
         <v>243</v>
       </c>
       <c r="G42" s="8" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="42.75">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>44</v>
       </c>
@@ -2639,10 +2649,10 @@
         <v>244</v>
       </c>
       <c r="G43" s="8" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>45</v>
       </c>
@@ -2656,10 +2666,10 @@
         <v>245</v>
       </c>
       <c r="G44" s="8" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>46</v>
       </c>
@@ -2673,10 +2683,10 @@
         <v>246</v>
       </c>
       <c r="G45" s="8" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="42.75">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>47</v>
       </c>
@@ -2690,10 +2700,10 @@
         <v>247</v>
       </c>
       <c r="G46" s="8" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>48</v>
       </c>
@@ -2707,10 +2717,10 @@
         <v>248</v>
       </c>
       <c r="G47" s="8" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>49</v>
       </c>
@@ -2724,10 +2734,10 @@
         <v>249</v>
       </c>
       <c r="G48" s="8" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="28.5">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>50</v>
       </c>
@@ -2741,10 +2751,10 @@
         <v>250</v>
       </c>
       <c r="G49" s="8" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="28.5">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>51</v>
       </c>
@@ -2758,10 +2768,10 @@
         <v>232</v>
       </c>
       <c r="G50" s="8" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="28.5">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>52</v>
       </c>
@@ -2775,10 +2785,10 @@
         <v>251</v>
       </c>
       <c r="G51" s="8" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>53</v>
       </c>
@@ -2795,7 +2805,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>54</v>
       </c>
@@ -2809,10 +2819,10 @@
         <v>253</v>
       </c>
       <c r="G53" s="8" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>55</v>
       </c>
@@ -2826,10 +2836,10 @@
         <v>254</v>
       </c>
       <c r="G54" s="8" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" ht="28.5">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>56</v>
       </c>
@@ -2843,10 +2853,10 @@
         <v>255</v>
       </c>
       <c r="G55" s="8" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" ht="28.5">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>57</v>
       </c>
@@ -2860,10 +2870,10 @@
         <v>256</v>
       </c>
       <c r="G56" s="8" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>58</v>
       </c>
@@ -2877,10 +2887,10 @@
         <v>257</v>
       </c>
       <c r="G57" s="8" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" ht="28.5">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>59</v>
       </c>
@@ -2894,10 +2904,10 @@
         <v>258</v>
       </c>
       <c r="G58" s="8" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>60</v>
       </c>
@@ -2911,10 +2921,10 @@
         <v>259</v>
       </c>
       <c r="G59" s="8" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" ht="28.5">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>61</v>
       </c>
@@ -2926,10 +2936,10 @@
         <v>260</v>
       </c>
       <c r="G60" s="8" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" ht="28.5">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>62</v>
       </c>
@@ -2943,10 +2953,10 @@
         <v>261</v>
       </c>
       <c r="G61" s="8" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" ht="28.5">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>63</v>
       </c>
@@ -2960,10 +2970,10 @@
         <v>262</v>
       </c>
       <c r="G62" s="8" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>64</v>
       </c>
@@ -2977,10 +2987,10 @@
         <v>263</v>
       </c>
       <c r="G63" s="8" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" ht="28.5">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>65</v>
       </c>
@@ -2994,10 +3004,10 @@
         <v>264</v>
       </c>
       <c r="G64" s="8" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>66</v>
       </c>
@@ -3011,10 +3021,10 @@
         <v>264</v>
       </c>
       <c r="G65" s="8" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>67</v>
       </c>
@@ -3028,10 +3038,10 @@
         <v>245</v>
       </c>
       <c r="G66" s="8" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>68</v>
       </c>
@@ -3048,7 +3058,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>69</v>
       </c>
@@ -3062,10 +3072,10 @@
         <v>205</v>
       </c>
       <c r="G68" s="8" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>70</v>
       </c>
@@ -3082,7 +3092,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>71</v>
       </c>
@@ -3096,10 +3106,10 @@
         <v>267</v>
       </c>
       <c r="G70" s="8" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>72</v>
       </c>
@@ -3113,10 +3123,10 @@
         <v>268</v>
       </c>
       <c r="G71" s="8" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>73</v>
       </c>
@@ -3130,10 +3140,10 @@
         <v>269</v>
       </c>
       <c r="G72" s="8" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>74</v>
       </c>
@@ -3147,10 +3157,10 @@
         <v>270</v>
       </c>
       <c r="G73" s="8" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" ht="28.5">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
         <v>75</v>
       </c>
@@ -3164,10 +3174,10 @@
         <v>271</v>
       </c>
       <c r="G74" s="8" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>76</v>
       </c>
@@ -3181,10 +3191,10 @@
         <v>272</v>
       </c>
       <c r="G75" s="8" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" ht="28.5">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
         <v>77</v>
       </c>
@@ -3198,10 +3208,10 @@
         <v>273</v>
       </c>
       <c r="G76" s="8" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" ht="28.5">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>78</v>
       </c>
@@ -3213,10 +3223,10 @@
         <v>274</v>
       </c>
       <c r="G77" s="8" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" ht="28.5">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>79</v>
       </c>
@@ -3230,10 +3240,10 @@
         <v>248</v>
       </c>
       <c r="G78" s="8" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>80</v>
       </c>
@@ -3247,10 +3257,10 @@
         <v>275</v>
       </c>
       <c r="G79" s="8" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>81</v>
       </c>
@@ -3264,10 +3274,10 @@
         <v>276</v>
       </c>
       <c r="G80" s="8" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" ht="28.5">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
         <v>82</v>
       </c>
@@ -3281,10 +3291,10 @@
         <v>277</v>
       </c>
       <c r="G81" s="8" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
         <v>83</v>
       </c>
@@ -3298,10 +3308,10 @@
         <v>278</v>
       </c>
       <c r="G82" s="8" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
         <v>84</v>
       </c>
@@ -3315,10 +3325,10 @@
         <v>279</v>
       </c>
       <c r="G83" s="8" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" ht="28.5">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>85</v>
       </c>
@@ -3332,10 +3342,10 @@
         <v>280</v>
       </c>
       <c r="G84" s="8" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
         <v>86</v>
       </c>
@@ -3349,10 +3359,10 @@
         <v>281</v>
       </c>
       <c r="G85" s="8" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
         <v>87</v>
       </c>
@@ -3366,10 +3376,10 @@
         <v>282</v>
       </c>
       <c r="G86" s="8" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
         <v>88</v>
       </c>
@@ -3383,10 +3393,10 @@
         <v>283</v>
       </c>
       <c r="G87" s="8" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
         <v>89</v>
       </c>
@@ -3400,10 +3410,10 @@
         <v>284</v>
       </c>
       <c r="G88" s="8" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" ht="28.5">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
         <v>118</v>
       </c>
@@ -3417,10 +3427,10 @@
         <v>285</v>
       </c>
       <c r="G89" s="8" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
         <v>115</v>
       </c>
@@ -3434,10 +3444,10 @@
         <v>287</v>
       </c>
       <c r="G90" s="8" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
         <v>90</v>
       </c>
@@ -3451,10 +3461,10 @@
         <v>288</v>
       </c>
       <c r="G91" s="8" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
         <v>91</v>
       </c>
@@ -3468,10 +3478,10 @@
         <v>289</v>
       </c>
       <c r="G92" s="8" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" ht="28.5">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
         <v>92</v>
       </c>
@@ -3485,10 +3495,10 @@
         <v>290</v>
       </c>
       <c r="G93" s="8" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" ht="28.5">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
         <v>116</v>
       </c>
@@ -3502,10 +3512,10 @@
         <v>291</v>
       </c>
       <c r="G94" s="8" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" ht="28.5">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
         <v>93</v>
       </c>
@@ -3519,10 +3529,10 @@
         <v>292</v>
       </c>
       <c r="G95" s="8" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
         <v>94</v>
       </c>
@@ -3536,10 +3546,10 @@
         <v>293</v>
       </c>
       <c r="G96" s="8" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
         <v>95</v>
       </c>
@@ -3553,10 +3563,10 @@
         <v>294</v>
       </c>
       <c r="G97" s="8" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
         <v>96</v>
       </c>
@@ -3570,10 +3580,10 @@
         <v>295</v>
       </c>
       <c r="G98" s="8" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" ht="28.5">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
         <v>97</v>
       </c>
@@ -3585,10 +3595,10 @@
         <v>296</v>
       </c>
       <c r="G99" s="8" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" ht="28.5">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
         <v>98</v>
       </c>
@@ -3602,10 +3612,10 @@
         <v>297</v>
       </c>
       <c r="G100" s="8" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" ht="28.5">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
         <v>99</v>
       </c>
@@ -3619,10 +3629,10 @@
         <v>297</v>
       </c>
       <c r="G101" s="8" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" ht="28.5">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
         <v>100</v>
       </c>
@@ -3636,10 +3646,10 @@
         <v>298</v>
       </c>
       <c r="G102" s="8" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
         <v>101</v>
       </c>
@@ -3653,10 +3663,10 @@
         <v>298</v>
       </c>
       <c r="G103" s="8" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
         <v>102</v>
       </c>
@@ -3670,10 +3680,10 @@
         <v>299</v>
       </c>
       <c r="G104" s="8" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
         <v>103</v>
       </c>
@@ -3687,10 +3697,10 @@
         <v>300</v>
       </c>
       <c r="G105" s="8" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" ht="42.75">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
         <v>104</v>
       </c>
@@ -3704,10 +3714,10 @@
         <v>301</v>
       </c>
       <c r="G106" s="8" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
         <v>105</v>
       </c>
@@ -3719,10 +3729,10 @@
         <v>302</v>
       </c>
       <c r="G107" s="8" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
         <v>106</v>
       </c>
@@ -3736,10 +3746,10 @@
         <v>303</v>
       </c>
       <c r="G108" s="8" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" ht="28.5">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
         <v>107</v>
       </c>
@@ -3753,10 +3763,10 @@
         <v>304</v>
       </c>
       <c r="G109" s="8" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
         <v>305</v>
       </c>
@@ -3773,7 +3783,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="111" spans="1:7" ht="28.5">
+    <row r="111" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
         <v>108</v>
       </c>
@@ -3787,10 +3797,10 @@
         <v>307</v>
       </c>
       <c r="G111" s="8" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
         <v>109</v>
       </c>
@@ -3804,10 +3814,10 @@
         <v>308</v>
       </c>
       <c r="G112" s="8" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7" ht="28.5">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
         <v>110</v>
       </c>
@@ -3821,10 +3831,10 @@
         <v>309</v>
       </c>
       <c r="G113" s="8" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="114" spans="1:7" ht="28.5">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
         <v>111</v>
       </c>
@@ -3838,10 +3848,10 @@
         <v>310</v>
       </c>
       <c r="G114" s="8" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="115" spans="1:7">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
         <v>112</v>
       </c>
@@ -3855,10 +3865,10 @@
         <v>311</v>
       </c>
       <c r="G115" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="116" spans="1:7" ht="28.5">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
         <v>113</v>
       </c>
@@ -3870,10 +3880,10 @@
         <v>312</v>
       </c>
       <c r="G116" s="8" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7" ht="42.75">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
         <v>114</v>
       </c>
@@ -3887,7 +3897,7 @@
         <v>313</v>
       </c>
       <c r="G117" s="8" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Small update to notes to translator.
</commit_message>
<xml_diff>
--- a/Trans Files/Master_Translation_All_Languages.xlsx
+++ b/Trans Files/Master_Translation_All_Languages.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="-75" yWindow="465" windowWidth="19320" windowHeight="12120"/>
@@ -2204,9 +2204,6 @@
     <t>Required for creating groups and finding friends. Your number is confidential and we will never expose it.</t>
   </si>
   <si>
-    <t>Info popup text describing why we need the phone number.</t>
-  </si>
-  <si>
     <t>נדרש עבור יצירת קבוצות ואיתור חברים. המספר שלך סודי ואנו לעולם לא נחשוף אותו.</t>
   </si>
   <si>
@@ -2263,13 +2260,16 @@
   </si>
   <si>
     <t>Feadback text</t>
+  </si>
+  <si>
+    <t>A small pop up information message that informs the user why we ask for his phone number</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2422,9 +2422,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="היפר-קישור" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="היפר-קישור שהופעל" xfId="2" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -2722,14 +2722,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="B179" sqref="B179"/>
+    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
+      <selection activeCell="C190" sqref="C190"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28.625" style="3" customWidth="1"/>
     <col min="2" max="2" width="55.625" style="1" customWidth="1"/>
@@ -2743,7 +2743,7 @@
     <col min="11" max="16384" width="8.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2775,12 +2775,12 @@
         <v>461</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="75">
+    <row r="2" spans="1:10" ht="75" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>649</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>416</v>
@@ -2803,7 +2803,7 @@
       </c>
       <c r="J2" s="4"/>
     </row>
-    <row r="3" spans="1:10" ht="30">
+    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
@@ -2827,7 +2827,7 @@
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
     </row>
-    <row r="4" spans="1:10" ht="30">
+    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>9</v>
       </c>
@@ -2855,7 +2855,7 @@
       </c>
       <c r="J4" s="4"/>
     </row>
-    <row r="5" spans="1:10" ht="60">
+    <row r="5" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>650</v>
       </c>
@@ -2879,7 +2879,7 @@
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
     </row>
-    <row r="6" spans="1:10" ht="15">
+    <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>10</v>
       </c>
@@ -2907,7 +2907,7 @@
       </c>
       <c r="J6" s="4"/>
     </row>
-    <row r="7" spans="1:10" ht="15">
+    <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>11</v>
       </c>
@@ -2935,7 +2935,7 @@
       </c>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="1:10" ht="15">
+    <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>12</v>
       </c>
@@ -2963,7 +2963,7 @@
       </c>
       <c r="J8" s="4"/>
     </row>
-    <row r="9" spans="1:10" ht="30">
+    <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>412</v>
       </c>
@@ -2991,7 +2991,7 @@
       </c>
       <c r="J9" s="4"/>
     </row>
-    <row r="10" spans="1:10" ht="15">
+    <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>13</v>
       </c>
@@ -3015,7 +3015,7 @@
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
     </row>
-    <row r="11" spans="1:10" ht="15">
+    <row r="11" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>516</v>
       </c>
@@ -3039,7 +3039,7 @@
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
     </row>
-    <row r="12" spans="1:10" ht="30">
+    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>14</v>
       </c>
@@ -3069,7 +3069,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="30">
+    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>203</v>
       </c>
@@ -3093,7 +3093,7 @@
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
     </row>
-    <row r="14" spans="1:10" ht="15">
+    <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>15</v>
       </c>
@@ -3117,7 +3117,7 @@
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
     </row>
-    <row r="15" spans="1:10" ht="15">
+    <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>16</v>
       </c>
@@ -3143,7 +3143,7 @@
       </c>
       <c r="J15" s="4"/>
     </row>
-    <row r="16" spans="1:10" ht="15">
+    <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
         <v>17</v>
       </c>
@@ -3167,7 +3167,7 @@
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
     </row>
-    <row r="17" spans="1:10" ht="15">
+    <row r="17" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
         <v>18</v>
       </c>
@@ -3191,7 +3191,7 @@
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
     </row>
-    <row r="18" spans="1:10" ht="15">
+    <row r="18" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
         <v>19</v>
       </c>
@@ -3215,7 +3215,7 @@
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
     </row>
-    <row r="19" spans="1:10" ht="15.75">
+    <row r="19" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>20</v>
       </c>
@@ -3243,7 +3243,7 @@
       </c>
       <c r="J19" s="4"/>
     </row>
-    <row r="20" spans="1:10" ht="15.75">
+    <row r="20" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>21</v>
       </c>
@@ -3271,7 +3271,7 @@
       </c>
       <c r="J20" s="4"/>
     </row>
-    <row r="21" spans="1:10" ht="15.75">
+    <row r="21" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>22</v>
       </c>
@@ -3299,7 +3299,7 @@
       </c>
       <c r="J21" s="4"/>
     </row>
-    <row r="22" spans="1:10" ht="30">
+    <row r="22" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A22" s="13" t="s">
         <v>411</v>
       </c>
@@ -3327,7 +3327,7 @@
       </c>
       <c r="J22" s="4"/>
     </row>
-    <row r="23" spans="1:10" ht="30">
+    <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
         <v>23</v>
       </c>
@@ -3357,7 +3357,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="30">
+    <row r="24" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
         <v>24</v>
       </c>
@@ -3381,7 +3381,7 @@
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
     </row>
-    <row r="25" spans="1:10" ht="15">
+    <row r="25" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
         <v>25</v>
       </c>
@@ -3405,7 +3405,7 @@
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
     </row>
-    <row r="26" spans="1:10" ht="15">
+    <row r="26" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
         <v>26</v>
       </c>
@@ -3433,7 +3433,7 @@
       </c>
       <c r="J26" s="4"/>
     </row>
-    <row r="27" spans="1:10" ht="15">
+    <row r="27" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
         <v>27</v>
       </c>
@@ -3463,7 +3463,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="15">
+    <row r="28" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
         <v>28</v>
       </c>
@@ -3493,7 +3493,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="30">
+    <row r="29" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
         <v>29</v>
       </c>
@@ -3517,7 +3517,7 @@
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
     </row>
-    <row r="30" spans="1:10" ht="15">
+    <row r="30" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
         <v>30</v>
       </c>
@@ -3541,7 +3541,7 @@
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
     </row>
-    <row r="31" spans="1:10" ht="15">
+    <row r="31" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
         <v>31</v>
       </c>
@@ -3565,7 +3565,7 @@
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
     </row>
-    <row r="32" spans="1:10" ht="15">
+    <row r="32" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
         <v>32</v>
       </c>
@@ -3595,7 +3595,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="45">
+    <row r="33" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
         <v>33</v>
       </c>
@@ -3623,7 +3623,7 @@
       </c>
       <c r="J33" s="4"/>
     </row>
-    <row r="34" spans="1:10" ht="15">
+    <row r="34" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
         <v>34</v>
       </c>
@@ -3647,7 +3647,7 @@
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
     </row>
-    <row r="35" spans="1:10" ht="15">
+    <row r="35" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
         <v>35</v>
       </c>
@@ -3675,7 +3675,7 @@
       </c>
       <c r="J35" s="4"/>
     </row>
-    <row r="36" spans="1:10" ht="15">
+    <row r="36" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A36" s="8" t="s">
         <v>36</v>
       </c>
@@ -3703,7 +3703,7 @@
       </c>
       <c r="J36" s="4"/>
     </row>
-    <row r="37" spans="1:10" ht="30">
+    <row r="37" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
         <v>227</v>
       </c>
@@ -3731,7 +3731,7 @@
       </c>
       <c r="J37" s="4"/>
     </row>
-    <row r="38" spans="1:10" ht="30">
+    <row r="38" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A38" s="8" t="s">
         <v>37</v>
       </c>
@@ -3755,7 +3755,7 @@
       <c r="I38" s="4"/>
       <c r="J38" s="4"/>
     </row>
-    <row r="39" spans="1:10" ht="15.75">
+    <row r="39" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
         <v>38</v>
       </c>
@@ -3783,7 +3783,7 @@
       </c>
       <c r="J39" s="4"/>
     </row>
-    <row r="40" spans="1:10" ht="15.75">
+    <row r="40" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
         <v>39</v>
       </c>
@@ -3811,7 +3811,7 @@
       </c>
       <c r="J40" s="4"/>
     </row>
-    <row r="41" spans="1:10" ht="30">
+    <row r="41" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A41" s="8" t="s">
         <v>112</v>
       </c>
@@ -3835,7 +3835,7 @@
       <c r="I41" s="4"/>
       <c r="J41" s="4"/>
     </row>
-    <row r="42" spans="1:10" ht="30">
+    <row r="42" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A42" s="8" t="s">
         <v>40</v>
       </c>
@@ -3859,7 +3859,7 @@
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
     </row>
-    <row r="43" spans="1:10" ht="45">
+    <row r="43" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
         <v>652</v>
       </c>
@@ -3887,7 +3887,7 @@
       </c>
       <c r="J43" s="4"/>
     </row>
-    <row r="44" spans="1:10" ht="15">
+    <row r="44" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A44" s="8" t="s">
         <v>41</v>
       </c>
@@ -3911,7 +3911,7 @@
       <c r="I44" s="4"/>
       <c r="J44" s="4"/>
     </row>
-    <row r="45" spans="1:10" ht="15.75">
+    <row r="45" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
         <v>42</v>
       </c>
@@ -3937,7 +3937,7 @@
       <c r="I45" s="4"/>
       <c r="J45" s="4"/>
     </row>
-    <row r="46" spans="1:10" ht="45">
+    <row r="46" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
         <v>43</v>
       </c>
@@ -3967,7 +3967,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="15">
+    <row r="47" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A47" s="8" t="s">
         <v>44</v>
       </c>
@@ -3991,7 +3991,7 @@
       <c r="I47" s="4"/>
       <c r="J47" s="4"/>
     </row>
-    <row r="48" spans="1:10" ht="15.75">
+    <row r="48" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
         <v>45</v>
       </c>
@@ -4019,7 +4019,7 @@
       </c>
       <c r="J48" s="4"/>
     </row>
-    <row r="49" spans="1:10" ht="30">
+    <row r="49" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A49" s="8" t="s">
         <v>46</v>
       </c>
@@ -4043,7 +4043,7 @@
       <c r="I49" s="4"/>
       <c r="J49" s="4"/>
     </row>
-    <row r="50" spans="1:10" ht="30">
+    <row r="50" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
         <v>47</v>
       </c>
@@ -4071,7 +4071,7 @@
       </c>
       <c r="J50" s="4"/>
     </row>
-    <row r="51" spans="1:10" ht="30">
+    <row r="51" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
         <v>48</v>
       </c>
@@ -4099,7 +4099,7 @@
       </c>
       <c r="J51" s="4"/>
     </row>
-    <row r="52" spans="1:10" ht="15.75">
+    <row r="52" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
         <v>49</v>
       </c>
@@ -4127,7 +4127,7 @@
       </c>
       <c r="J52" s="4"/>
     </row>
-    <row r="53" spans="1:10" ht="15">
+    <row r="53" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A53" s="8" t="s">
         <v>50</v>
       </c>
@@ -4151,7 +4151,7 @@
       <c r="I53" s="4"/>
       <c r="J53" s="4"/>
     </row>
-    <row r="54" spans="1:10" ht="30">
+    <row r="54" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A54" s="8" t="s">
         <v>51</v>
       </c>
@@ -4175,7 +4175,7 @@
       <c r="I54" s="4"/>
       <c r="J54" s="4"/>
     </row>
-    <row r="55" spans="1:10" ht="30">
+    <row r="55" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A55" s="8" t="s">
         <v>52</v>
       </c>
@@ -4199,7 +4199,7 @@
       <c r="I55" s="4"/>
       <c r="J55" s="4"/>
     </row>
-    <row r="56" spans="1:10" ht="30">
+    <row r="56" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A56" s="8" t="s">
         <v>53</v>
       </c>
@@ -4223,7 +4223,7 @@
       <c r="I56" s="4"/>
       <c r="J56" s="4"/>
     </row>
-    <row r="57" spans="1:10" ht="15.75">
+    <row r="57" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="8" t="s">
         <v>54</v>
       </c>
@@ -4251,7 +4251,7 @@
       </c>
       <c r="J57" s="4"/>
     </row>
-    <row r="58" spans="1:10" ht="30">
+    <row r="58" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A58" s="8" t="s">
         <v>55</v>
       </c>
@@ -4275,7 +4275,7 @@
       <c r="I58" s="4"/>
       <c r="J58" s="4"/>
     </row>
-    <row r="59" spans="1:10" ht="15">
+    <row r="59" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A59" s="8" t="s">
         <v>56</v>
       </c>
@@ -4299,7 +4299,7 @@
       <c r="I59" s="4"/>
       <c r="J59" s="4"/>
     </row>
-    <row r="60" spans="1:10" ht="30">
+    <row r="60" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A60" s="8" t="s">
         <v>57</v>
       </c>
@@ -4321,7 +4321,7 @@
       <c r="I60" s="4"/>
       <c r="J60" s="4"/>
     </row>
-    <row r="61" spans="1:10" ht="30">
+    <row r="61" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A61" s="8" t="s">
         <v>58</v>
       </c>
@@ -4345,7 +4345,7 @@
       <c r="I61" s="4"/>
       <c r="J61" s="4"/>
     </row>
-    <row r="62" spans="1:10" ht="30">
+    <row r="62" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A62" s="8" t="s">
         <v>59</v>
       </c>
@@ -4373,7 +4373,7 @@
       </c>
       <c r="J62" s="4"/>
     </row>
-    <row r="63" spans="1:10" ht="15">
+    <row r="63" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A63" s="8" t="s">
         <v>60</v>
       </c>
@@ -4397,7 +4397,7 @@
       <c r="I63" s="4"/>
       <c r="J63" s="4"/>
     </row>
-    <row r="64" spans="1:10" ht="30">
+    <row r="64" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="8" t="s">
         <v>61</v>
       </c>
@@ -4425,7 +4425,7 @@
       </c>
       <c r="J64" s="4"/>
     </row>
-    <row r="65" spans="1:10" ht="15">
+    <row r="65" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A65" s="8" t="s">
         <v>62</v>
       </c>
@@ -4453,7 +4453,7 @@
       </c>
       <c r="J65" s="4"/>
     </row>
-    <row r="66" spans="1:10" ht="15.75">
+    <row r="66" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="8" t="s">
         <v>63</v>
       </c>
@@ -4481,7 +4481,7 @@
       </c>
       <c r="J66" s="4"/>
     </row>
-    <row r="67" spans="1:10" ht="15">
+    <row r="67" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A67" s="8" t="s">
         <v>64</v>
       </c>
@@ -4505,7 +4505,7 @@
       <c r="I67" s="4"/>
       <c r="J67" s="4"/>
     </row>
-    <row r="68" spans="1:10" ht="15.75">
+    <row r="68" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="8" t="s">
         <v>65</v>
       </c>
@@ -4533,7 +4533,7 @@
       </c>
       <c r="J68" s="4"/>
     </row>
-    <row r="69" spans="1:10" ht="15">
+    <row r="69" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A69" s="8" t="s">
         <v>66</v>
       </c>
@@ -4557,7 +4557,7 @@
       <c r="I69" s="4"/>
       <c r="J69" s="4"/>
     </row>
-    <row r="70" spans="1:10" ht="15">
+    <row r="70" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A70" s="8" t="s">
         <v>67</v>
       </c>
@@ -4581,7 +4581,7 @@
       <c r="I70" s="4"/>
       <c r="J70" s="4"/>
     </row>
-    <row r="71" spans="1:10" ht="15.75">
+    <row r="71" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="8" t="s">
         <v>68</v>
       </c>
@@ -4609,7 +4609,7 @@
       </c>
       <c r="J71" s="4"/>
     </row>
-    <row r="72" spans="1:10" ht="15.75">
+    <row r="72" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="8" t="s">
         <v>69</v>
       </c>
@@ -4637,7 +4637,7 @@
       </c>
       <c r="J72" s="4"/>
     </row>
-    <row r="73" spans="1:10" ht="15">
+    <row r="73" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A73" s="8" t="s">
         <v>70</v>
       </c>
@@ -4665,7 +4665,7 @@
       </c>
       <c r="J73" s="4"/>
     </row>
-    <row r="74" spans="1:10" ht="30">
+    <row r="74" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A74" s="8" t="s">
         <v>71</v>
       </c>
@@ -4693,7 +4693,7 @@
       </c>
       <c r="J74" s="4"/>
     </row>
-    <row r="75" spans="1:10" ht="15">
+    <row r="75" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A75" s="8" t="s">
         <v>72</v>
       </c>
@@ -4721,7 +4721,7 @@
       </c>
       <c r="J75" s="4"/>
     </row>
-    <row r="76" spans="1:10" ht="30">
+    <row r="76" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A76" s="8" t="s">
         <v>73</v>
       </c>
@@ -4745,7 +4745,7 @@
       <c r="I76" s="4"/>
       <c r="J76" s="4"/>
     </row>
-    <row r="77" spans="1:10" ht="45">
+    <row r="77" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A77" s="8" t="s">
         <v>74</v>
       </c>
@@ -4767,7 +4767,7 @@
       <c r="I77" s="4"/>
       <c r="J77" s="4"/>
     </row>
-    <row r="78" spans="1:10" ht="30">
+    <row r="78" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A78" s="8" t="s">
         <v>75</v>
       </c>
@@ -4791,7 +4791,7 @@
       <c r="I78" s="4"/>
       <c r="J78" s="4"/>
     </row>
-    <row r="79" spans="1:10" ht="15.75">
+    <row r="79" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="8" t="s">
         <v>76</v>
       </c>
@@ -4819,7 +4819,7 @@
       </c>
       <c r="J79" s="4"/>
     </row>
-    <row r="80" spans="1:10" ht="15.75">
+    <row r="80" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="8" t="s">
         <v>77</v>
       </c>
@@ -4849,7 +4849,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="15.75">
+    <row r="81" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="8" t="s">
         <v>78</v>
       </c>
@@ -4877,7 +4877,7 @@
       </c>
       <c r="J81" s="4"/>
     </row>
-    <row r="82" spans="1:10" ht="15">
+    <row r="82" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A82" s="8" t="s">
         <v>79</v>
       </c>
@@ -4907,7 +4907,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="83" spans="1:10" ht="15">
+    <row r="83" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A83" s="8" t="s">
         <v>80</v>
       </c>
@@ -4935,7 +4935,7 @@
       </c>
       <c r="J83" s="4"/>
     </row>
-    <row r="84" spans="1:10" ht="30">
+    <row r="84" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="8" t="s">
         <v>81</v>
       </c>
@@ -4965,7 +4965,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="85" spans="1:10" ht="15.75">
+    <row r="85" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="8" t="s">
         <v>82</v>
       </c>
@@ -4993,7 +4993,7 @@
       </c>
       <c r="J85" s="4"/>
     </row>
-    <row r="86" spans="1:10" ht="15">
+    <row r="86" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A86" s="8" t="s">
         <v>83</v>
       </c>
@@ -5017,7 +5017,7 @@
       <c r="I86" s="4"/>
       <c r="J86" s="4"/>
     </row>
-    <row r="87" spans="1:10" ht="15">
+    <row r="87" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A87" s="8" t="s">
         <v>84</v>
       </c>
@@ -5041,7 +5041,7 @@
       <c r="I87" s="4"/>
       <c r="J87" s="4"/>
     </row>
-    <row r="88" spans="1:10" ht="15">
+    <row r="88" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A88" s="8" t="s">
         <v>85</v>
       </c>
@@ -5065,7 +5065,7 @@
       <c r="I88" s="4"/>
       <c r="J88" s="4"/>
     </row>
-    <row r="89" spans="1:10" ht="30">
+    <row r="89" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="8" t="s">
         <v>113</v>
       </c>
@@ -5093,7 +5093,7 @@
       </c>
       <c r="J89" s="4"/>
     </row>
-    <row r="90" spans="1:10" ht="15.75">
+    <row r="90" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90" s="8" t="s">
         <v>110</v>
       </c>
@@ -5121,7 +5121,7 @@
       </c>
       <c r="J90" s="4"/>
     </row>
-    <row r="91" spans="1:10" ht="15.75">
+    <row r="91" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91" s="8" t="s">
         <v>86</v>
       </c>
@@ -5147,7 +5147,7 @@
       </c>
       <c r="J91" s="4"/>
     </row>
-    <row r="92" spans="1:10" ht="30">
+    <row r="92" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A92" s="8" t="s">
         <v>87</v>
       </c>
@@ -5175,7 +5175,7 @@
       </c>
       <c r="J92" s="4"/>
     </row>
-    <row r="93" spans="1:10" ht="30">
+    <row r="93" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A93" s="8" t="s">
         <v>88</v>
       </c>
@@ -5203,7 +5203,7 @@
       </c>
       <c r="J93" s="4"/>
     </row>
-    <row r="94" spans="1:10" ht="30">
+    <row r="94" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A94" s="8" t="s">
         <v>111</v>
       </c>
@@ -5231,7 +5231,7 @@
       </c>
       <c r="J94" s="4"/>
     </row>
-    <row r="95" spans="1:10" ht="30">
+    <row r="95" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A95" s="8" t="s">
         <v>89</v>
       </c>
@@ -5255,7 +5255,7 @@
       <c r="I95" s="4"/>
       <c r="J95" s="4"/>
     </row>
-    <row r="96" spans="1:10" ht="15">
+    <row r="96" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A96" s="8" t="s">
         <v>90</v>
       </c>
@@ -5279,7 +5279,7 @@
       <c r="I96" s="4"/>
       <c r="J96" s="4"/>
     </row>
-    <row r="97" spans="1:10" ht="15.75">
+    <row r="97" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A97" s="8" t="s">
         <v>91</v>
       </c>
@@ -5307,7 +5307,7 @@
       </c>
       <c r="J97" s="4"/>
     </row>
-    <row r="98" spans="1:10" ht="15">
+    <row r="98" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A98" s="8" t="s">
         <v>92</v>
       </c>
@@ -5337,7 +5337,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="99" spans="1:10" ht="30">
+    <row r="99" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A99" s="8" t="s">
         <v>93</v>
       </c>
@@ -5365,7 +5365,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="100" spans="1:10" ht="30">
+    <row r="100" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A100" s="8" t="s">
         <v>94</v>
       </c>
@@ -5395,7 +5395,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="101" spans="1:10" ht="30">
+    <row r="101" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A101" s="8" t="s">
         <v>95</v>
       </c>
@@ -5423,7 +5423,7 @@
       </c>
       <c r="J101" s="4"/>
     </row>
-    <row r="102" spans="1:10" ht="30">
+    <row r="102" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A102" s="8" t="s">
         <v>96</v>
       </c>
@@ -5451,7 +5451,7 @@
       </c>
       <c r="J102" s="4"/>
     </row>
-    <row r="103" spans="1:10" ht="15">
+    <row r="103" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A103" s="8" t="s">
         <v>97</v>
       </c>
@@ -5479,7 +5479,7 @@
       </c>
       <c r="J103" s="4"/>
     </row>
-    <row r="104" spans="1:10" ht="15">
+    <row r="104" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A104" s="8" t="s">
         <v>98</v>
       </c>
@@ -5503,7 +5503,7 @@
       <c r="I104" s="4"/>
       <c r="J104" s="4"/>
     </row>
-    <row r="105" spans="1:10" ht="15">
+    <row r="105" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A105" s="8" t="s">
         <v>99</v>
       </c>
@@ -5527,7 +5527,7 @@
       <c r="I105" s="4"/>
       <c r="J105" s="4"/>
     </row>
-    <row r="106" spans="1:10" ht="30">
+    <row r="106" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A106" s="8" t="s">
         <v>100</v>
       </c>
@@ -5551,7 +5551,7 @@
       <c r="I106" s="4"/>
       <c r="J106" s="4"/>
     </row>
-    <row r="107" spans="1:10" ht="15">
+    <row r="107" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A107" s="8" t="s">
         <v>101</v>
       </c>
@@ -5573,7 +5573,7 @@
       <c r="I107" s="4"/>
       <c r="J107" s="4"/>
     </row>
-    <row r="108" spans="1:10" ht="15">
+    <row r="108" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A108" s="8" t="s">
         <v>102</v>
       </c>
@@ -5599,7 +5599,7 @@
       <c r="I108" s="4"/>
       <c r="J108" s="4"/>
     </row>
-    <row r="109" spans="1:10" ht="30">
+    <row r="109" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A109" s="8" t="s">
         <v>103</v>
       </c>
@@ -5623,7 +5623,7 @@
       <c r="I109" s="4"/>
       <c r="J109" s="4"/>
     </row>
-    <row r="110" spans="1:10" ht="15">
+    <row r="110" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A110" s="8" t="s">
         <v>296</v>
       </c>
@@ -5647,7 +5647,7 @@
       <c r="I110" s="4"/>
       <c r="J110" s="4"/>
     </row>
-    <row r="111" spans="1:10" ht="30">
+    <row r="111" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A111" s="8" t="s">
         <v>104</v>
       </c>
@@ -5675,7 +5675,7 @@
       </c>
       <c r="J111" s="4"/>
     </row>
-    <row r="112" spans="1:10" ht="15">
+    <row r="112" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A112" s="8" t="s">
         <v>105</v>
       </c>
@@ -5703,7 +5703,7 @@
       </c>
       <c r="J112" s="4"/>
     </row>
-    <row r="113" spans="1:10" ht="30">
+    <row r="113" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A113" s="8" t="s">
         <v>106</v>
       </c>
@@ -5727,7 +5727,7 @@
       <c r="I113" s="4"/>
       <c r="J113" s="4"/>
     </row>
-    <row r="114" spans="1:10" ht="15">
+    <row r="114" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A114" s="8" t="s">
         <v>107</v>
       </c>
@@ -5755,7 +5755,7 @@
       </c>
       <c r="J114" s="4"/>
     </row>
-    <row r="115" spans="1:10" ht="15">
+    <row r="115" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A115" s="8" t="s">
         <v>108</v>
       </c>
@@ -5783,7 +5783,7 @@
       </c>
       <c r="J115" s="4"/>
     </row>
-    <row r="116" spans="1:10" ht="30">
+    <row r="116" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A116" s="8" t="s">
         <v>109</v>
       </c>
@@ -5805,7 +5805,7 @@
       <c r="I116" s="4"/>
       <c r="J116" s="4"/>
     </row>
-    <row r="117" spans="1:10" ht="45">
+    <row r="117" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A117" s="8" t="s">
         <v>654</v>
       </c>
@@ -5829,9 +5829,9 @@
       <c r="I117" s="4"/>
       <c r="J117" s="4"/>
     </row>
-    <row r="118" spans="1:10" ht="30">
+    <row r="118" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A118" s="23" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B118" s="24"/>
       <c r="C118" s="25" t="s">
@@ -5853,7 +5853,7 @@
       </c>
       <c r="J118" s="12"/>
     </row>
-    <row r="119" spans="1:10" ht="15.75">
+    <row r="119" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A119" s="11" t="s">
         <v>33</v>
       </c>
@@ -5877,9 +5877,9 @@
       </c>
       <c r="J119" s="12"/>
     </row>
-    <row r="120" spans="1:10" ht="15.75">
+    <row r="120" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A120" s="17" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B120" s="12"/>
       <c r="C120" s="16" t="s">
@@ -5892,7 +5892,7 @@
         <v>108</v>
       </c>
       <c r="F120" s="22" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="G120" s="12"/>
       <c r="H120" s="12"/>
@@ -5901,7 +5901,7 @@
       </c>
       <c r="J120" s="12"/>
     </row>
-    <row r="121" spans="1:10" ht="15.75">
+    <row r="121" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A121" s="11" t="s">
         <v>700</v>
       </c>
@@ -5916,7 +5916,7 @@
         <v>108</v>
       </c>
       <c r="F121" s="22" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="G121" s="12"/>
       <c r="H121" s="12"/>
@@ -5925,7 +5925,7 @@
       </c>
       <c r="J121" s="12"/>
     </row>
-    <row r="122" spans="1:10" ht="15.75">
+    <row r="122" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A122" s="11" t="s">
         <v>695</v>
       </c>
@@ -5949,7 +5949,7 @@
       </c>
       <c r="J122" s="12"/>
     </row>
-    <row r="123" spans="1:10" ht="15.75">
+    <row r="123" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A123" s="17" t="s">
         <v>701</v>
       </c>
@@ -5964,7 +5964,7 @@
         <v>108</v>
       </c>
       <c r="F123" s="22" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="G123" s="12"/>
       <c r="H123" s="12"/>
@@ -5973,7 +5973,7 @@
       </c>
       <c r="J123" s="12"/>
     </row>
-    <row r="124" spans="1:10" ht="15.75">
+    <row r="124" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A124" s="11" t="s">
         <v>696</v>
       </c>
@@ -5997,7 +5997,7 @@
       </c>
       <c r="J124" s="12"/>
     </row>
-    <row r="125" spans="1:10" ht="30">
+    <row r="125" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A125" s="11" t="s">
         <v>698</v>
       </c>
@@ -6021,9 +6021,9 @@
       </c>
       <c r="J125" s="12"/>
     </row>
-    <row r="126" spans="1:10" ht="15.75">
+    <row r="126" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A126" s="17" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="B126" s="24"/>
       <c r="C126" s="25" t="s">
@@ -6036,7 +6036,7 @@
         <v>108</v>
       </c>
       <c r="F126" s="22" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="G126" s="12"/>
       <c r="H126" s="12"/>
@@ -6045,7 +6045,7 @@
       </c>
       <c r="J126" s="12"/>
     </row>
-    <row r="127" spans="1:10" ht="45">
+    <row r="127" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A127" s="11" t="s">
         <v>699</v>
       </c>
@@ -6069,7 +6069,7 @@
       </c>
       <c r="J127" s="12"/>
     </row>
-    <row r="128" spans="1:10" ht="15.75">
+    <row r="128" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A128" s="11" t="s">
         <v>697</v>
       </c>
@@ -6093,9 +6093,9 @@
       </c>
       <c r="J128" s="12"/>
     </row>
-    <row r="129" spans="1:10" ht="15.75">
+    <row r="129" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A129" s="11" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B129" s="12"/>
       <c r="C129" s="16" t="s">
@@ -6117,7 +6117,7 @@
       </c>
       <c r="J129" s="12"/>
     </row>
-    <row r="130" spans="1:10" ht="45">
+    <row r="130" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A130" s="11" t="s">
         <v>682</v>
       </c>
@@ -6141,7 +6141,7 @@
       </c>
       <c r="J130" s="12"/>
     </row>
-    <row r="131" spans="1:10" ht="15.75">
+    <row r="131" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A131" s="11" t="s">
         <v>683</v>
       </c>
@@ -6165,7 +6165,7 @@
       </c>
       <c r="J131" s="12"/>
     </row>
-    <row r="132" spans="1:10" ht="30">
+    <row r="132" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A132" s="11" t="s">
         <v>684</v>
       </c>
@@ -6189,7 +6189,7 @@
       </c>
       <c r="J132" s="12"/>
     </row>
-    <row r="133" spans="1:10" ht="30">
+    <row r="133" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A133" s="11" t="s">
         <v>658</v>
       </c>
@@ -6213,7 +6213,7 @@
       </c>
       <c r="J133" s="12"/>
     </row>
-    <row r="134" spans="1:10" ht="15.75">
+    <row r="134" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A134" s="11" t="s">
         <v>659</v>
       </c>
@@ -6237,7 +6237,7 @@
       </c>
       <c r="J134" s="12"/>
     </row>
-    <row r="135" spans="1:10" ht="15.75">
+    <row r="135" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A135" s="11" t="s">
         <v>660</v>
       </c>
@@ -6261,7 +6261,7 @@
       </c>
       <c r="J135" s="12"/>
     </row>
-    <row r="136" spans="1:10" ht="15.75">
+    <row r="136" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A136" s="11" t="s">
         <v>21</v>
       </c>
@@ -6285,7 +6285,7 @@
       </c>
       <c r="J136" s="12"/>
     </row>
-    <row r="137" spans="1:10" ht="15.75">
+    <row r="137" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A137" s="11" t="s">
         <v>661</v>
       </c>
@@ -6309,7 +6309,7 @@
       </c>
       <c r="J137" s="12"/>
     </row>
-    <row r="138" spans="1:10" ht="15.75">
+    <row r="138" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A138" s="11" t="s">
         <v>16</v>
       </c>
@@ -6333,7 +6333,7 @@
       </c>
       <c r="J138" s="12"/>
     </row>
-    <row r="139" spans="1:10" ht="75">
+    <row r="139" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A139" s="11" t="s">
         <v>675</v>
       </c>
@@ -6357,7 +6357,7 @@
       </c>
       <c r="J139" s="12"/>
     </row>
-    <row r="140" spans="1:10" ht="15.75">
+    <row r="140" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A140" s="11" t="s">
         <v>662</v>
       </c>
@@ -6381,7 +6381,7 @@
       </c>
       <c r="J140" s="12"/>
     </row>
-    <row r="141" spans="1:10" ht="30">
+    <row r="141" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A141" s="11" t="s">
         <v>663</v>
       </c>
@@ -6405,7 +6405,7 @@
       </c>
       <c r="J141" s="12"/>
     </row>
-    <row r="142" spans="1:10" ht="15.75">
+    <row r="142" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A142" s="11" t="s">
         <v>664</v>
       </c>
@@ -6429,7 +6429,7 @@
       </c>
       <c r="J142" s="12"/>
     </row>
-    <row r="143" spans="1:10" ht="15.75">
+    <row r="143" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A143" s="11" t="s">
         <v>64</v>
       </c>
@@ -6453,7 +6453,7 @@
       </c>
       <c r="J143" s="12"/>
     </row>
-    <row r="144" spans="1:10" ht="30">
+    <row r="144" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A144" s="11" t="s">
         <v>73</v>
       </c>
@@ -6477,7 +6477,7 @@
       </c>
       <c r="J144" s="12"/>
     </row>
-    <row r="145" spans="1:10" ht="30">
+    <row r="145" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A145" s="11" t="s">
         <v>667</v>
       </c>
@@ -6501,7 +6501,7 @@
       </c>
       <c r="J145" s="12"/>
     </row>
-    <row r="146" spans="1:10" ht="30">
+    <row r="146" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A146" s="11" t="s">
         <v>668</v>
       </c>
@@ -6525,7 +6525,7 @@
       </c>
       <c r="J146" s="12"/>
     </row>
-    <row r="147" spans="1:10" ht="15.75">
+    <row r="147" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A147" s="11" t="s">
         <v>21</v>
       </c>
@@ -6549,7 +6549,7 @@
       </c>
       <c r="J147" s="12"/>
     </row>
-    <row r="148" spans="1:10" ht="15.75">
+    <row r="148" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A148" s="11" t="s">
         <v>16</v>
       </c>
@@ -6573,7 +6573,7 @@
       </c>
       <c r="J148" s="12"/>
     </row>
-    <row r="149" spans="1:10" ht="15.75">
+    <row r="149" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A149" s="11" t="s">
         <v>676</v>
       </c>
@@ -6597,9 +6597,9 @@
       </c>
       <c r="J149" s="12"/>
     </row>
-    <row r="150" spans="1:10" ht="15.75">
+    <row r="150" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A150" s="17" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B150" s="12"/>
       <c r="C150" s="16" t="s">
@@ -6621,7 +6621,7 @@
       </c>
       <c r="J150" s="12"/>
     </row>
-    <row r="151" spans="1:10" ht="15.75">
+    <row r="151" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A151" s="11" t="s">
         <v>671</v>
       </c>
@@ -6645,7 +6645,7 @@
       </c>
       <c r="J151" s="12"/>
     </row>
-    <row r="152" spans="1:10" ht="15.75">
+    <row r="152" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A152" s="11" t="s">
         <v>666</v>
       </c>
@@ -6669,7 +6669,7 @@
       </c>
       <c r="J152" s="12"/>
     </row>
-    <row r="153" spans="1:10" ht="15.75">
+    <row r="153" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A153" s="11" t="s">
         <v>677</v>
       </c>
@@ -6693,7 +6693,7 @@
       </c>
       <c r="J153" s="12"/>
     </row>
-    <row r="154" spans="1:10" ht="30">
+    <row r="154" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A154" s="11" t="s">
         <v>669</v>
       </c>
@@ -6717,7 +6717,7 @@
       </c>
       <c r="J154" s="12"/>
     </row>
-    <row r="155" spans="1:10" ht="15.75">
+    <row r="155" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A155" s="11" t="s">
         <v>670</v>
       </c>
@@ -6741,7 +6741,7 @@
       </c>
       <c r="J155" s="12"/>
     </row>
-    <row r="156" spans="1:10" ht="15.75">
+    <row r="156" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A156" s="11" t="s">
         <v>678</v>
       </c>
@@ -6765,7 +6765,7 @@
       </c>
       <c r="J156" s="12"/>
     </row>
-    <row r="157" spans="1:10" ht="15.75">
+    <row r="157" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A157" s="11" t="s">
         <v>665</v>
       </c>
@@ -6789,7 +6789,7 @@
       </c>
       <c r="J157" s="12"/>
     </row>
-    <row r="158" spans="1:10" ht="15.75">
+    <row r="158" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A158" s="11" t="s">
         <v>672</v>
       </c>
@@ -6813,7 +6813,7 @@
       </c>
       <c r="J158" s="12"/>
     </row>
-    <row r="159" spans="1:10" ht="15.75">
+    <row r="159" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A159" s="11" t="s">
         <v>673</v>
       </c>
@@ -6837,7 +6837,7 @@
       </c>
       <c r="J159" s="12"/>
     </row>
-    <row r="160" spans="1:10" ht="15.75">
+    <row r="160" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A160" s="11" t="s">
         <v>51</v>
       </c>
@@ -6861,7 +6861,7 @@
       </c>
       <c r="J160" s="12"/>
     </row>
-    <row r="161" spans="1:10" ht="15.75">
+    <row r="161" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A161" s="11" t="s">
         <v>674</v>
       </c>
@@ -6885,7 +6885,7 @@
       </c>
       <c r="J161" s="12"/>
     </row>
-    <row r="162" spans="1:10" ht="15.75">
+    <row r="162" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A162" s="11" t="s">
         <v>679</v>
       </c>
@@ -6909,7 +6909,7 @@
       </c>
       <c r="J162" s="12"/>
     </row>
-    <row r="163" spans="1:10" ht="15.75">
+    <row r="163" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A163" s="11" t="s">
         <v>680</v>
       </c>
@@ -6933,7 +6933,7 @@
       </c>
       <c r="J163" s="12"/>
     </row>
-    <row r="164" spans="1:10" ht="15.75">
+    <row r="164" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A164" s="11" t="s">
         <v>681</v>
       </c>
@@ -6957,7 +6957,7 @@
       </c>
       <c r="J164" s="12"/>
     </row>
-    <row r="165" spans="1:10" ht="15.75">
+    <row r="165" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A165" s="11" t="s">
         <v>685</v>
       </c>
@@ -6981,7 +6981,7 @@
       </c>
       <c r="J165" s="12"/>
     </row>
-    <row r="166" spans="1:10" ht="15">
+    <row r="166" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A166" s="11" t="s">
         <v>42</v>
       </c>
@@ -7005,7 +7005,7 @@
       </c>
       <c r="J166" s="12"/>
     </row>
-    <row r="167" spans="1:10" ht="15.75">
+    <row r="167" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A167" s="11" t="s">
         <v>686</v>
       </c>
@@ -7029,7 +7029,7 @@
       </c>
       <c r="J167" s="12"/>
     </row>
-    <row r="168" spans="1:10" ht="30">
+    <row r="168" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A168" s="11" t="s">
         <v>687</v>
       </c>
@@ -7053,7 +7053,7 @@
       </c>
       <c r="J168" s="12"/>
     </row>
-    <row r="169" spans="1:10" ht="15.75">
+    <row r="169" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A169" s="11" t="s">
         <v>688</v>
       </c>
@@ -7077,7 +7077,7 @@
       </c>
       <c r="J169" s="12"/>
     </row>
-    <row r="170" spans="1:10" ht="30">
+    <row r="170" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A170" s="11" t="s">
         <v>689</v>
       </c>
@@ -7101,7 +7101,7 @@
       </c>
       <c r="J170" s="12"/>
     </row>
-    <row r="171" spans="1:10" ht="15.75">
+    <row r="171" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A171" s="11" t="s">
         <v>690</v>
       </c>
@@ -7125,7 +7125,7 @@
       </c>
       <c r="J171" s="12"/>
     </row>
-    <row r="172" spans="1:10" ht="45">
+    <row r="172" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A172" s="11" t="s">
         <v>691</v>
       </c>
@@ -7149,7 +7149,7 @@
       </c>
       <c r="J172" s="12"/>
     </row>
-    <row r="173" spans="1:10" ht="15.75">
+    <row r="173" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A173" s="11" t="s">
         <v>690</v>
       </c>
@@ -7173,7 +7173,7 @@
       </c>
       <c r="J173" s="12"/>
     </row>
-    <row r="174" spans="1:10" ht="15.75">
+    <row r="174" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A174" s="11" t="s">
         <v>692</v>
       </c>
@@ -7197,7 +7197,7 @@
       </c>
       <c r="J174" s="12"/>
     </row>
-    <row r="175" spans="1:10" ht="15.75">
+    <row r="175" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A175" s="11" t="s">
         <v>702</v>
       </c>
@@ -7221,7 +7221,7 @@
       </c>
       <c r="J175" s="12"/>
     </row>
-    <row r="176" spans="1:10" ht="15.75">
+    <row r="176" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A176" s="11" t="s">
         <v>52</v>
       </c>
@@ -7245,7 +7245,7 @@
       </c>
       <c r="J176" s="12"/>
     </row>
-    <row r="177" spans="1:10" ht="15.75">
+    <row r="177" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A177" s="11" t="s">
         <v>693</v>
       </c>
@@ -7269,9 +7269,9 @@
       </c>
       <c r="J177" s="12"/>
     </row>
-    <row r="178" spans="1:10" ht="15.75">
+    <row r="178" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A178" s="17" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B178" s="12"/>
       <c r="C178" s="16" t="s">
@@ -7293,7 +7293,7 @@
       </c>
       <c r="J178" s="12"/>
     </row>
-    <row r="179" spans="1:10" ht="15.75">
+    <row r="179" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A179" s="11" t="s">
         <v>694</v>
       </c>
@@ -7315,9 +7315,9 @@
       <c r="I179" s="12"/>
       <c r="J179" s="12"/>
     </row>
-    <row r="180" spans="1:10" ht="15.75">
+    <row r="180" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A180" s="17" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="B180" s="12"/>
       <c r="C180" s="16" t="s">
@@ -7330,14 +7330,14 @@
         <v>108</v>
       </c>
       <c r="F180" s="13" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="G180" s="12"/>
       <c r="H180" s="12"/>
       <c r="I180" s="12"/>
       <c r="J180" s="12"/>
     </row>
-    <row r="181" spans="1:10" ht="15.75">
+    <row r="181" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A181" s="11" t="s">
         <v>21</v>
       </c>
@@ -7359,7 +7359,7 @@
       <c r="I181" s="12"/>
       <c r="J181" s="12"/>
     </row>
-    <row r="182" spans="1:10">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A182" s="19" t="s">
         <v>703</v>
       </c>
@@ -7381,7 +7381,7 @@
       <c r="I182" s="20"/>
       <c r="J182" s="20"/>
     </row>
-    <row r="183" spans="1:10">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A183" s="19" t="s">
         <v>707</v>
       </c>
@@ -7403,7 +7403,7 @@
       <c r="I183" s="20"/>
       <c r="J183" s="20"/>
     </row>
-    <row r="184" spans="1:10">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A184" s="19" t="s">
         <v>711</v>
       </c>
@@ -7425,7 +7425,7 @@
       <c r="I184" s="20"/>
       <c r="J184" s="20"/>
     </row>
-    <row r="185" spans="1:10">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A185" s="19" t="s">
         <v>713</v>
       </c>
@@ -7447,7 +7447,7 @@
       <c r="I185" s="20"/>
       <c r="J185" s="20"/>
     </row>
-    <row r="186" spans="1:10">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A186" s="19" t="s">
         <v>715</v>
       </c>
@@ -7469,7 +7469,7 @@
       <c r="I186" s="20"/>
       <c r="J186" s="20"/>
     </row>
-    <row r="187" spans="1:10">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A187" s="19" t="s">
         <v>718</v>
       </c>
@@ -7491,7 +7491,7 @@
       <c r="I187" s="20"/>
       <c r="J187" s="20"/>
     </row>
-    <row r="188" spans="1:10">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A188" s="19" t="s">
         <v>720</v>
       </c>
@@ -7513,7 +7513,7 @@
       <c r="I188" s="20"/>
       <c r="J188" s="20"/>
     </row>
-    <row r="189" spans="1:10">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A189" s="19" t="s">
         <v>722</v>
       </c>
@@ -7535,12 +7535,12 @@
       <c r="I189" s="20"/>
       <c r="J189" s="20"/>
     </row>
-    <row r="190" spans="1:10" ht="57">
+    <row r="190" spans="1:10" ht="57" x14ac:dyDescent="0.2">
       <c r="A190" s="19" t="s">
         <v>724</v>
       </c>
-      <c r="B190" s="20" t="s">
-        <v>725</v>
+      <c r="B190" s="19" t="s">
+        <v>744</v>
       </c>
       <c r="C190" s="20"/>
       <c r="D190" s="21" t="s">
@@ -7550,19 +7550,19 @@
         <v>705</v>
       </c>
       <c r="F190" s="19" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="G190" s="20"/>
       <c r="H190" s="20"/>
       <c r="I190" s="20"/>
       <c r="J190" s="20"/>
     </row>
-    <row r="191" spans="1:10">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A191" s="19" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B191" s="20" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="C191" s="20"/>
       <c r="D191" s="21" t="s">
@@ -7572,19 +7572,19 @@
         <v>705</v>
       </c>
       <c r="F191" s="19" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="G191" s="20"/>
       <c r="H191" s="20"/>
       <c r="I191" s="20"/>
       <c r="J191" s="20"/>
     </row>
-    <row r="192" spans="1:10">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A192" s="19" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B192" s="20" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="C192" s="20"/>
       <c r="D192" s="21" t="s">
@@ -7594,7 +7594,7 @@
         <v>705</v>
       </c>
       <c r="F192" s="19" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="G192" s="20"/>
       <c r="H192" s="20"/>

</xml_diff>

<commit_message>
Made changes to existing translation
</commit_message>
<xml_diff>
--- a/Trans Files/Master_Translation_All_Languages.xlsx
+++ b/Trans Files/Master_Translation_All_Languages.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1277" uniqueCount="745">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1278" uniqueCount="744">
   <si>
     <t>Source (English)</t>
   </si>
@@ -1257,9 +1257,6 @@
   </si>
   <si>
     <t>absenden</t>
-  </si>
-  <si>
-    <t>Collect</t>
   </si>
   <si>
     <t>Address Selector</t>
@@ -2725,8 +2722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
-      <selection activeCell="C190" sqref="C190"/>
+    <sheetView tabSelected="1" topLeftCell="B82" workbookViewId="0">
+      <selection activeCell="B88" sqref="B88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2769,21 +2766,21 @@
         <v>7</v>
       </c>
       <c r="I1" s="6" t="s">
+        <v>459</v>
+      </c>
+      <c r="J1" s="15" t="s">
         <v>460</v>
-      </c>
-      <c r="J1" s="15" t="s">
-        <v>461</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="75" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>108</v>
@@ -2799,7 +2796,7 @@
       </c>
       <c r="H2" s="12"/>
       <c r="I2" s="4" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="J2" s="4"/>
     </row>
@@ -2835,7 +2832,7 @@
         <v>307</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>108</v>
@@ -2851,16 +2848,16 @@
       </c>
       <c r="H4" s="12"/>
       <c r="I4" s="4" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="J4" s="4"/>
     </row>
     <row r="5" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
+        <v>649</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>650</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>651</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="9" t="s">
@@ -2887,7 +2884,7 @@
         <v>116</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>108</v>
@@ -2903,7 +2900,7 @@
       </c>
       <c r="H6" s="12"/>
       <c r="I6" s="4" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="J6" s="4"/>
     </row>
@@ -2915,7 +2912,7 @@
         <v>117</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>108</v>
@@ -2931,7 +2928,7 @@
       </c>
       <c r="H7" s="12"/>
       <c r="I7" s="4" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="J7" s="4"/>
     </row>
@@ -2943,7 +2940,7 @@
         <v>118</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>108</v>
@@ -2959,35 +2956,35 @@
       </c>
       <c r="H8" s="12"/>
       <c r="I8" s="4" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="J8" s="4"/>
     </row>
     <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
+        <v>411</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>413</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="F9" s="10" t="s">
         <v>412</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>414</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>421</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>413</v>
       </c>
       <c r="G9" s="17" t="s">
         <v>382</v>
       </c>
       <c r="H9" s="12"/>
       <c r="I9" s="4" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="J9" s="4"/>
     </row>
@@ -3017,10 +3014,10 @@
     </row>
     <row r="11" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="9" t="s">
@@ -3047,7 +3044,7 @@
         <v>120</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>108</v>
@@ -3063,10 +3060,10 @@
       </c>
       <c r="H12" s="12"/>
       <c r="I12" s="4" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.2">
@@ -3102,7 +3099,7 @@
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="9" t="s">
-        <v>108</v>
+        <v>54</v>
       </c>
       <c r="E14" s="18" t="s">
         <v>54</v>
@@ -3139,7 +3136,7 @@
       </c>
       <c r="H15" s="12"/>
       <c r="I15" s="4" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="J15" s="4"/>
     </row>
@@ -3223,7 +3220,7 @@
         <v>125</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D19" s="9" t="s">
         <v>108</v>
@@ -3239,7 +3236,7 @@
       </c>
       <c r="H19" s="12"/>
       <c r="I19" s="4" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="J19" s="4"/>
     </row>
@@ -3251,7 +3248,7 @@
         <v>126</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D20" s="9" t="s">
         <v>108</v>
@@ -3267,7 +3264,7 @@
       </c>
       <c r="H20" s="12"/>
       <c r="I20" s="4" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="J20" s="4"/>
     </row>
@@ -3279,7 +3276,7 @@
         <v>115</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D21" s="9" t="s">
         <v>108</v>
@@ -3295,19 +3292,19 @@
       </c>
       <c r="H21" s="12"/>
       <c r="I21" s="4" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="J21" s="4"/>
     </row>
     <row r="22" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A22" s="13" t="s">
-        <v>411</v>
+        <v>69</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D22" s="9" t="s">
         <v>108</v>
@@ -3319,11 +3316,11 @@
         <v>260</v>
       </c>
       <c r="G22" s="17" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="H22" s="12"/>
       <c r="I22" s="4" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="J22" s="4"/>
     </row>
@@ -3335,7 +3332,7 @@
         <v>127</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D23" s="9" t="s">
         <v>108</v>
@@ -3351,10 +3348,10 @@
       </c>
       <c r="H23" s="12"/>
       <c r="I23" s="4" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="30" x14ac:dyDescent="0.2">
@@ -3413,7 +3410,7 @@
         <v>130</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D26" s="9" t="s">
         <v>108</v>
@@ -3429,7 +3426,7 @@
       </c>
       <c r="H26" s="12"/>
       <c r="I26" s="4" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="J26" s="4"/>
     </row>
@@ -3441,7 +3438,7 @@
         <v>131</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D27" s="9" t="s">
         <v>108</v>
@@ -3457,10 +3454,10 @@
       </c>
       <c r="H27" s="12"/>
       <c r="I27" s="4" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="15" x14ac:dyDescent="0.2">
@@ -3471,7 +3468,7 @@
         <v>132</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D28" s="9" t="s">
         <v>108</v>
@@ -3487,10 +3484,10 @@
       </c>
       <c r="H28" s="12"/>
       <c r="I28" s="4" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="30" x14ac:dyDescent="0.2">
@@ -3573,7 +3570,7 @@
         <v>131</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D32" s="9" t="s">
         <v>108</v>
@@ -3589,10 +3586,10 @@
       </c>
       <c r="H32" s="12"/>
       <c r="I32" s="4" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="45" x14ac:dyDescent="0.2">
@@ -3603,7 +3600,7 @@
         <v>135</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D33" s="9" t="s">
         <v>108</v>
@@ -3619,7 +3616,7 @@
       </c>
       <c r="H33" s="12"/>
       <c r="I33" s="4" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="J33" s="4"/>
     </row>
@@ -3655,7 +3652,7 @@
         <v>115</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D35" s="9" t="s">
         <v>108</v>
@@ -3671,7 +3668,7 @@
       </c>
       <c r="H35" s="12"/>
       <c r="I35" s="4" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="J35" s="4"/>
     </row>
@@ -3683,7 +3680,7 @@
         <v>137</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D36" s="9" t="s">
         <v>108</v>
@@ -3699,7 +3696,7 @@
       </c>
       <c r="H36" s="12"/>
       <c r="I36" s="4" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="J36" s="4"/>
     </row>
@@ -3711,7 +3708,7 @@
         <v>228</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D37" s="9" t="s">
         <v>108</v>
@@ -3723,11 +3720,11 @@
         <v>306</v>
       </c>
       <c r="G37" s="17" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="H37" s="12"/>
       <c r="I37" s="4" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="J37" s="4"/>
     </row>
@@ -3763,7 +3760,7 @@
         <v>139</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="D39" s="9" t="s">
         <v>108</v>
@@ -3779,7 +3776,7 @@
       </c>
       <c r="H39" s="12"/>
       <c r="I39" s="4" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="J39" s="4"/>
     </row>
@@ -3791,7 +3788,7 @@
         <v>140</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D40" s="9" t="s">
         <v>108</v>
@@ -3807,7 +3804,7 @@
       </c>
       <c r="H40" s="12"/>
       <c r="I40" s="4" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="J40" s="4"/>
     </row>
@@ -3861,19 +3858,19 @@
     </row>
     <row r="43" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
+        <v>651</v>
+      </c>
+      <c r="B43" s="8" t="s">
         <v>652</v>
       </c>
-      <c r="B43" s="8" t="s">
-        <v>653</v>
-      </c>
       <c r="C43" s="16" t="s">
+        <v>471</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="E43" s="18" t="s">
         <v>472</v>
-      </c>
-      <c r="D43" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="E43" s="18" t="s">
-        <v>473</v>
       </c>
       <c r="F43" s="10" t="s">
         <v>235</v>
@@ -3883,7 +3880,7 @@
       </c>
       <c r="H43" s="12"/>
       <c r="I43" s="4" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="J43" s="4"/>
     </row>
@@ -3899,7 +3896,7 @@
         <v>108</v>
       </c>
       <c r="E44" s="18" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="F44" s="10" t="s">
         <v>236</v>
@@ -3919,7 +3916,7 @@
         <v>143</v>
       </c>
       <c r="C45" s="16" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D45" s="9" t="s">
         <v>108</v>
@@ -3945,7 +3942,7 @@
         <v>119</v>
       </c>
       <c r="C46" s="16" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="D46" s="9" t="s">
         <v>108</v>
@@ -3961,10 +3958,10 @@
       </c>
       <c r="H46" s="12"/>
       <c r="I46" s="4" t="s">
+        <v>487</v>
+      </c>
+      <c r="J46" s="4" t="s">
         <v>488</v>
-      </c>
-      <c r="J46" s="4" t="s">
-        <v>489</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="15" x14ac:dyDescent="0.2">
@@ -3999,7 +3996,7 @@
         <v>145</v>
       </c>
       <c r="C48" s="16" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D48" s="9" t="s">
         <v>108</v>
@@ -4015,7 +4012,7 @@
       </c>
       <c r="H48" s="12"/>
       <c r="I48" s="4" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="J48" s="4"/>
     </row>
@@ -4051,7 +4048,7 @@
         <v>146</v>
       </c>
       <c r="C50" s="16" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D50" s="9" t="s">
         <v>108</v>
@@ -4067,7 +4064,7 @@
       </c>
       <c r="H50" s="12"/>
       <c r="I50" s="4" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="J50" s="4"/>
     </row>
@@ -4079,7 +4076,7 @@
         <v>147</v>
       </c>
       <c r="C51" s="16" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="D51" s="9" t="s">
         <v>108</v>
@@ -4095,7 +4092,7 @@
       </c>
       <c r="H51" s="12"/>
       <c r="I51" s="4" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="J51" s="4"/>
     </row>
@@ -4107,7 +4104,7 @@
         <v>148</v>
       </c>
       <c r="C52" s="16" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="D52" s="9" t="s">
         <v>108</v>
@@ -4123,7 +4120,7 @@
       </c>
       <c r="H52" s="12"/>
       <c r="I52" s="4" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="J52" s="4"/>
     </row>
@@ -4231,7 +4228,7 @@
         <v>126</v>
       </c>
       <c r="C57" s="16" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D57" s="9" t="s">
         <v>108</v>
@@ -4247,7 +4244,7 @@
       </c>
       <c r="H57" s="12"/>
       <c r="I57" s="4" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="J57" s="4"/>
     </row>
@@ -4353,7 +4350,7 @@
         <v>156</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D62" s="9" t="s">
         <v>108</v>
@@ -4369,7 +4366,7 @@
       </c>
       <c r="H62" s="12"/>
       <c r="I62" s="4" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="J62" s="4"/>
     </row>
@@ -4405,7 +4402,7 @@
         <v>158</v>
       </c>
       <c r="C64" s="16" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D64" s="9" t="s">
         <v>108</v>
@@ -4421,7 +4418,7 @@
       </c>
       <c r="H64" s="12"/>
       <c r="I64" s="4" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="J64" s="4"/>
     </row>
@@ -4433,7 +4430,7 @@
         <v>159</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D65" s="9" t="s">
         <v>108</v>
@@ -4449,7 +4446,7 @@
       </c>
       <c r="H65" s="12"/>
       <c r="I65" s="4" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="J65" s="4"/>
     </row>
@@ -4461,7 +4458,7 @@
         <v>115</v>
       </c>
       <c r="C66" s="16" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="D66" s="9" t="s">
         <v>108</v>
@@ -4477,7 +4474,7 @@
       </c>
       <c r="H66" s="12"/>
       <c r="I66" s="4" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="J66" s="4"/>
     </row>
@@ -4513,7 +4510,7 @@
         <v>115</v>
       </c>
       <c r="C68" s="16" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D68" s="9" t="s">
         <v>108</v>
@@ -4529,7 +4526,7 @@
       </c>
       <c r="H68" s="12"/>
       <c r="I68" s="4" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="J68" s="4"/>
     </row>
@@ -4589,7 +4586,7 @@
         <v>162</v>
       </c>
       <c r="C71" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="D71" s="9" t="s">
         <v>108</v>
@@ -4605,7 +4602,7 @@
       </c>
       <c r="H71" s="12"/>
       <c r="I71" s="4" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="J71" s="4"/>
     </row>
@@ -4617,7 +4614,7 @@
         <v>163</v>
       </c>
       <c r="C72" s="16" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D72" s="9" t="s">
         <v>108</v>
@@ -4633,7 +4630,7 @@
       </c>
       <c r="H72" s="12"/>
       <c r="I72" s="4" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="J72" s="4"/>
     </row>
@@ -4645,7 +4642,7 @@
         <v>164</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D73" s="9" t="s">
         <v>108</v>
@@ -4661,7 +4658,7 @@
       </c>
       <c r="H73" s="12"/>
       <c r="I73" s="4" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="J73" s="4"/>
     </row>
@@ -4673,7 +4670,7 @@
         <v>165</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D74" s="9" t="s">
         <v>108</v>
@@ -4689,7 +4686,7 @@
       </c>
       <c r="H74" s="12"/>
       <c r="I74" s="4" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="J74" s="4"/>
     </row>
@@ -4701,7 +4698,7 @@
         <v>166</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D75" s="9" t="s">
         <v>108</v>
@@ -4717,7 +4714,7 @@
       </c>
       <c r="H75" s="12"/>
       <c r="I75" s="4" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="J75" s="4"/>
     </row>
@@ -4799,7 +4796,7 @@
         <v>115</v>
       </c>
       <c r="C79" s="16" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D79" s="9" t="s">
         <v>108</v>
@@ -4815,7 +4812,7 @@
       </c>
       <c r="H79" s="12"/>
       <c r="I79" s="4" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="J79" s="4"/>
     </row>
@@ -4827,7 +4824,7 @@
         <v>168</v>
       </c>
       <c r="C80" s="16" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D80" s="9" t="s">
         <v>108</v>
@@ -4843,10 +4840,10 @@
       </c>
       <c r="H80" s="12"/>
       <c r="I80" s="4" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="J80" s="4" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="81" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -4857,7 +4854,7 @@
         <v>127</v>
       </c>
       <c r="C81" s="16" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D81" s="9" t="s">
         <v>108</v>
@@ -4873,7 +4870,7 @@
       </c>
       <c r="H81" s="12"/>
       <c r="I81" s="4" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="J81" s="4"/>
     </row>
@@ -4885,7 +4882,7 @@
         <v>169</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D82" s="9" t="s">
         <v>108</v>
@@ -4901,10 +4898,10 @@
       </c>
       <c r="H82" s="12"/>
       <c r="I82" s="4" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="J82" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="83" spans="1:10" ht="15" x14ac:dyDescent="0.2">
@@ -4915,7 +4912,7 @@
         <v>161</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D83" s="9" t="s">
         <v>108</v>
@@ -4931,7 +4928,7 @@
       </c>
       <c r="H83" s="12"/>
       <c r="I83" s="4" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="J83" s="4"/>
     </row>
@@ -4943,7 +4940,7 @@
         <v>170</v>
       </c>
       <c r="C84" s="16" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D84" s="9" t="s">
         <v>108</v>
@@ -4959,7 +4956,7 @@
       </c>
       <c r="H84" s="12"/>
       <c r="I84" s="4" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="J84" s="4" t="s">
         <v>294</v>
@@ -4973,7 +4970,7 @@
         <v>171</v>
       </c>
       <c r="C85" s="16" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D85" s="9" t="s">
         <v>108</v>
@@ -4989,7 +4986,7 @@
       </c>
       <c r="H85" s="12"/>
       <c r="I85" s="4" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="J85" s="4"/>
     </row>
@@ -5073,7 +5070,7 @@
         <v>277</v>
       </c>
       <c r="C89" s="16" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D89" s="9" t="s">
         <v>108</v>
@@ -5089,7 +5086,7 @@
       </c>
       <c r="H89" s="12"/>
       <c r="I89" s="4" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="J89" s="4"/>
     </row>
@@ -5101,7 +5098,7 @@
         <v>192</v>
       </c>
       <c r="C90" s="16" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D90" s="9" t="s">
         <v>108</v>
@@ -5117,7 +5114,7 @@
       </c>
       <c r="H90" s="12"/>
       <c r="I90" s="4" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="J90" s="4"/>
     </row>
@@ -5143,7 +5140,7 @@
       </c>
       <c r="H91" s="12"/>
       <c r="I91" s="4" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="J91" s="4"/>
     </row>
@@ -5155,7 +5152,7 @@
         <v>176</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D92" s="9" t="s">
         <v>108</v>
@@ -5171,7 +5168,7 @@
       </c>
       <c r="H92" s="12"/>
       <c r="I92" s="4" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="J92" s="4"/>
     </row>
@@ -5183,7 +5180,7 @@
         <v>177</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D93" s="9" t="s">
         <v>108</v>
@@ -5199,7 +5196,7 @@
       </c>
       <c r="H93" s="12"/>
       <c r="I93" s="4" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="J93" s="4"/>
     </row>
@@ -5211,7 +5208,7 @@
         <v>193</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D94" s="9" t="s">
         <v>108</v>
@@ -5227,7 +5224,7 @@
       </c>
       <c r="H94" s="12"/>
       <c r="I94" s="4" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="J94" s="4"/>
     </row>
@@ -5287,7 +5284,7 @@
         <v>180</v>
       </c>
       <c r="C97" s="16" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D97" s="9" t="s">
         <v>108</v>
@@ -5303,7 +5300,7 @@
       </c>
       <c r="H97" s="12"/>
       <c r="I97" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="J97" s="4"/>
     </row>
@@ -5315,7 +5312,7 @@
         <v>131</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D98" s="9" t="s">
         <v>108</v>
@@ -5331,10 +5328,10 @@
       </c>
       <c r="H98" s="12"/>
       <c r="I98" s="4" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="J98" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="99" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -5343,7 +5340,7 @@
       </c>
       <c r="B99" s="8"/>
       <c r="C99" s="16" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="D99" s="9" t="s">
         <v>108</v>
@@ -5359,10 +5356,10 @@
       </c>
       <c r="H99" s="12"/>
       <c r="I99" s="4" t="s">
+        <v>487</v>
+      </c>
+      <c r="J99" s="4" t="s">
         <v>488</v>
-      </c>
-      <c r="J99" s="4" t="s">
-        <v>489</v>
       </c>
     </row>
     <row r="100" spans="1:10" ht="30" x14ac:dyDescent="0.2">
@@ -5373,7 +5370,7 @@
         <v>181</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D100" s="9" t="s">
         <v>108</v>
@@ -5389,10 +5386,10 @@
       </c>
       <c r="H100" s="12"/>
       <c r="I100" s="4" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="J100" s="4" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="101" spans="1:10" ht="30" x14ac:dyDescent="0.2">
@@ -5403,7 +5400,7 @@
         <v>182</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D101" s="9" t="s">
         <v>108</v>
@@ -5419,7 +5416,7 @@
       </c>
       <c r="H101" s="12"/>
       <c r="I101" s="4" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="J101" s="4"/>
     </row>
@@ -5431,7 +5428,7 @@
         <v>183</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D102" s="9" t="s">
         <v>108</v>
@@ -5447,7 +5444,7 @@
       </c>
       <c r="H102" s="12"/>
       <c r="I102" s="4" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="J102" s="4"/>
     </row>
@@ -5459,7 +5456,7 @@
         <v>184</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D103" s="9" t="s">
         <v>108</v>
@@ -5475,7 +5472,7 @@
       </c>
       <c r="H103" s="12"/>
       <c r="I103" s="4" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="J103" s="4"/>
     </row>
@@ -5581,7 +5578,7 @@
         <v>186</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="D108" s="9" t="s">
         <v>108</v>
@@ -5655,7 +5652,7 @@
         <v>188</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D111" s="9" t="s">
         <v>108</v>
@@ -5671,7 +5668,7 @@
       </c>
       <c r="H111" s="12"/>
       <c r="I111" s="4" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="J111" s="4"/>
     </row>
@@ -5683,7 +5680,7 @@
         <v>189</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D112" s="9" t="s">
         <v>108</v>
@@ -5699,7 +5696,7 @@
       </c>
       <c r="H112" s="12"/>
       <c r="I112" s="4" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="J112" s="4"/>
     </row>
@@ -5735,7 +5732,7 @@
         <v>191</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D114" s="9" t="s">
         <v>108</v>
@@ -5751,7 +5748,7 @@
       </c>
       <c r="H114" s="12"/>
       <c r="I114" s="4" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="J114" s="4"/>
     </row>
@@ -5763,7 +5760,7 @@
         <v>126</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D115" s="9" t="s">
         <v>108</v>
@@ -5779,7 +5776,7 @@
       </c>
       <c r="H115" s="12"/>
       <c r="I115" s="4" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="J115" s="4"/>
     </row>
@@ -5807,10 +5804,10 @@
     </row>
     <row r="117" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A117" s="8" t="s">
+        <v>653</v>
+      </c>
+      <c r="B117" s="8" t="s">
         <v>654</v>
-      </c>
-      <c r="B117" s="8" t="s">
-        <v>655</v>
       </c>
       <c r="C117" s="4"/>
       <c r="D117" s="9" t="s">
@@ -5831,25 +5828,25 @@
     </row>
     <row r="118" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A118" s="23" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B118" s="24"/>
       <c r="C118" s="25" t="s">
+        <v>516</v>
+      </c>
+      <c r="D118" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="E118" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="F118" s="22" t="s">
         <v>517</v>
-      </c>
-      <c r="D118" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="E118" s="26" t="s">
-        <v>108</v>
-      </c>
-      <c r="F118" s="22" t="s">
-        <v>518</v>
       </c>
       <c r="G118" s="12"/>
       <c r="H118" s="12"/>
       <c r="I118" s="12" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="J118" s="12"/>
     </row>
@@ -5859,7 +5856,7 @@
       </c>
       <c r="B119" s="12"/>
       <c r="C119" s="16" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D119" s="9" t="s">
         <v>54</v>
@@ -5873,17 +5870,17 @@
       <c r="G119" s="12"/>
       <c r="H119" s="12"/>
       <c r="I119" s="12" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="J119" s="12"/>
     </row>
     <row r="120" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A120" s="17" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="B120" s="12"/>
       <c r="C120" s="16" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="D120" s="9" t="s">
         <v>54</v>
@@ -5892,22 +5889,22 @@
         <v>108</v>
       </c>
       <c r="F120" s="22" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="G120" s="12"/>
       <c r="H120" s="12"/>
       <c r="I120" s="12" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="J120" s="12"/>
     </row>
     <row r="121" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A121" s="11" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="B121" s="12"/>
       <c r="C121" s="16" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="D121" s="9" t="s">
         <v>54</v>
@@ -5916,46 +5913,46 @@
         <v>108</v>
       </c>
       <c r="F121" s="22" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="G121" s="12"/>
       <c r="H121" s="12"/>
       <c r="I121" s="12" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="J121" s="12"/>
     </row>
     <row r="122" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A122" s="11" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="B122" s="12"/>
       <c r="C122" s="16" t="s">
+        <v>522</v>
+      </c>
+      <c r="D122" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E122" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F122" s="13" t="s">
         <v>523</v>
-      </c>
-      <c r="D122" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E122" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="F122" s="13" t="s">
-        <v>524</v>
       </c>
       <c r="G122" s="12"/>
       <c r="H122" s="12"/>
       <c r="I122" s="12" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="J122" s="12"/>
     </row>
     <row r="123" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A123" s="17" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="B123" s="12"/>
       <c r="C123" s="16" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D123" s="9" t="s">
         <v>54</v>
@@ -5964,46 +5961,46 @@
         <v>108</v>
       </c>
       <c r="F123" s="22" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="G123" s="12"/>
       <c r="H123" s="12"/>
       <c r="I123" s="12" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="J123" s="12"/>
     </row>
     <row r="124" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A124" s="11" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="B124" s="12"/>
       <c r="C124" s="16" t="s">
+        <v>526</v>
+      </c>
+      <c r="D124" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E124" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F124" s="13" t="s">
         <v>527</v>
-      </c>
-      <c r="D124" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E124" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="F124" s="13" t="s">
-        <v>528</v>
       </c>
       <c r="G124" s="12"/>
       <c r="H124" s="12"/>
       <c r="I124" s="12" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="J124" s="12"/>
     </row>
     <row r="125" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A125" s="11" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="B125" s="12"/>
       <c r="C125" s="16" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="D125" s="9" t="s">
         <v>54</v>
@@ -6012,22 +6009,22 @@
         <v>108</v>
       </c>
       <c r="F125" s="13" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="G125" s="12"/>
       <c r="H125" s="12"/>
       <c r="I125" s="12" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="J125" s="12"/>
     </row>
     <row r="126" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A126" s="17" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B126" s="24"/>
       <c r="C126" s="25" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="D126" s="26" t="s">
         <v>54</v>
@@ -6036,94 +6033,94 @@
         <v>108</v>
       </c>
       <c r="F126" s="22" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="G126" s="12"/>
       <c r="H126" s="12"/>
       <c r="I126" s="12" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="J126" s="12"/>
     </row>
     <row r="127" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A127" s="11" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="B127" s="12"/>
       <c r="C127" s="16" t="s">
+        <v>573</v>
+      </c>
+      <c r="D127" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E127" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F127" s="13" t="s">
         <v>574</v>
-      </c>
-      <c r="D127" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E127" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="F127" s="13" t="s">
-        <v>575</v>
       </c>
       <c r="G127" s="12"/>
       <c r="H127" s="12"/>
       <c r="I127" s="12" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="J127" s="12"/>
     </row>
     <row r="128" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A128" s="11" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="B128" s="12"/>
       <c r="C128" s="16" t="s">
+        <v>532</v>
+      </c>
+      <c r="D128" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E128" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F128" s="13" t="s">
         <v>533</v>
-      </c>
-      <c r="D128" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E128" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="F128" s="13" t="s">
-        <v>534</v>
       </c>
       <c r="G128" s="12"/>
       <c r="H128" s="12"/>
       <c r="I128" s="12" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="J128" s="12"/>
     </row>
     <row r="129" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A129" s="11" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B129" s="12"/>
       <c r="C129" s="16" t="s">
+        <v>535</v>
+      </c>
+      <c r="D129" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E129" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F129" s="13" t="s">
         <v>536</v>
-      </c>
-      <c r="D129" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E129" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="F129" s="13" t="s">
-        <v>537</v>
       </c>
       <c r="G129" s="12"/>
       <c r="H129" s="12"/>
       <c r="I129" s="12" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="J129" s="12"/>
     </row>
     <row r="130" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A130" s="11" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="B130" s="12"/>
       <c r="C130" s="16" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="D130" s="9" t="s">
         <v>54</v>
@@ -6132,70 +6129,70 @@
         <v>108</v>
       </c>
       <c r="F130" s="13" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="G130" s="12"/>
       <c r="H130" s="12"/>
       <c r="I130" s="12" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="J130" s="12"/>
     </row>
     <row r="131" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A131" s="11" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B131" s="12"/>
       <c r="C131" s="16" t="s">
+        <v>539</v>
+      </c>
+      <c r="D131" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E131" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F131" s="13" t="s">
         <v>540</v>
-      </c>
-      <c r="D131" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E131" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="F131" s="13" t="s">
-        <v>541</v>
       </c>
       <c r="G131" s="12"/>
       <c r="H131" s="12"/>
       <c r="I131" s="12" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="J131" s="12"/>
     </row>
     <row r="132" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A132" s="11" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="B132" s="12"/>
       <c r="C132" s="16" t="s">
+        <v>541</v>
+      </c>
+      <c r="D132" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E132" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F132" s="13" t="s">
         <v>542</v>
-      </c>
-      <c r="D132" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E132" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="F132" s="13" t="s">
-        <v>543</v>
       </c>
       <c r="G132" s="12"/>
       <c r="H132" s="12"/>
       <c r="I132" s="12" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="J132" s="12"/>
     </row>
     <row r="133" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A133" s="11" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="B133" s="12"/>
       <c r="C133" s="16" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="D133" s="9" t="s">
         <v>54</v>
@@ -6204,22 +6201,22 @@
         <v>108</v>
       </c>
       <c r="F133" s="13" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G133" s="12"/>
       <c r="H133" s="12"/>
       <c r="I133" s="12" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="J133" s="12"/>
     </row>
     <row r="134" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A134" s="11" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="B134" s="12"/>
       <c r="C134" s="16" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="D134" s="9" t="s">
         <v>54</v>
@@ -6228,36 +6225,36 @@
         <v>108</v>
       </c>
       <c r="F134" s="13" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="G134" s="12"/>
       <c r="H134" s="12"/>
       <c r="I134" s="12" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="J134" s="12"/>
     </row>
     <row r="135" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A135" s="11" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B135" s="12"/>
       <c r="C135" s="16" t="s">
+        <v>547</v>
+      </c>
+      <c r="D135" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E135" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F135" s="13" t="s">
         <v>548</v>
-      </c>
-      <c r="D135" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E135" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="F135" s="13" t="s">
-        <v>549</v>
       </c>
       <c r="G135" s="12"/>
       <c r="H135" s="12"/>
       <c r="I135" s="12" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="J135" s="12"/>
     </row>
@@ -6267,7 +6264,7 @@
       </c>
       <c r="B136" s="12"/>
       <c r="C136" s="16" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="D136" s="9" t="s">
         <v>54</v>
@@ -6276,36 +6273,36 @@
         <v>108</v>
       </c>
       <c r="F136" s="13" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="G136" s="12"/>
       <c r="H136" s="12"/>
       <c r="I136" s="12" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="J136" s="12"/>
     </row>
     <row r="137" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A137" s="11" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B137" s="12"/>
       <c r="C137" s="16" t="s">
+        <v>551</v>
+      </c>
+      <c r="D137" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E137" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F137" s="13" t="s">
         <v>552</v>
-      </c>
-      <c r="D137" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E137" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="F137" s="13" t="s">
-        <v>553</v>
       </c>
       <c r="G137" s="12"/>
       <c r="H137" s="12"/>
       <c r="I137" s="12" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="J137" s="12"/>
     </row>
@@ -6315,7 +6312,7 @@
       </c>
       <c r="B138" s="12"/>
       <c r="C138" s="16" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D138" s="9" t="s">
         <v>54</v>
@@ -6329,103 +6326,103 @@
       <c r="G138" s="12"/>
       <c r="H138" s="12"/>
       <c r="I138" s="12" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="J138" s="12"/>
     </row>
     <row r="139" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A139" s="11" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B139" s="12"/>
       <c r="C139" s="16" t="s">
+        <v>554</v>
+      </c>
+      <c r="D139" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E139" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F139" s="13" t="s">
         <v>555</v>
-      </c>
-      <c r="D139" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E139" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="F139" s="13" t="s">
-        <v>556</v>
       </c>
       <c r="G139" s="12"/>
       <c r="H139" s="12"/>
       <c r="I139" s="12" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="J139" s="12"/>
     </row>
     <row r="140" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A140" s="11" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B140" s="12"/>
       <c r="C140" s="16" t="s">
+        <v>556</v>
+      </c>
+      <c r="D140" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E140" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F140" s="13" t="s">
         <v>557</v>
-      </c>
-      <c r="D140" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E140" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="F140" s="13" t="s">
-        <v>558</v>
       </c>
       <c r="G140" s="12"/>
       <c r="H140" s="12"/>
       <c r="I140" s="12" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="J140" s="12"/>
     </row>
     <row r="141" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A141" s="11" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="B141" s="12"/>
       <c r="C141" s="16" t="s">
+        <v>559</v>
+      </c>
+      <c r="D141" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E141" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F141" s="13" t="s">
         <v>560</v>
-      </c>
-      <c r="D141" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E141" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="F141" s="13" t="s">
-        <v>561</v>
       </c>
       <c r="G141" s="12"/>
       <c r="H141" s="12"/>
       <c r="I141" s="12" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="J141" s="12"/>
     </row>
     <row r="142" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A142" s="11" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="B142" s="12"/>
       <c r="C142" s="16" t="s">
+        <v>561</v>
+      </c>
+      <c r="D142" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E142" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F142" s="13" t="s">
         <v>562</v>
-      </c>
-      <c r="D142" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E142" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="F142" s="13" t="s">
-        <v>563</v>
       </c>
       <c r="G142" s="12"/>
       <c r="H142" s="12"/>
       <c r="I142" s="12" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="J142" s="12"/>
     </row>
@@ -6435,7 +6432,7 @@
       </c>
       <c r="B143" s="12"/>
       <c r="C143" s="16" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="D143" s="9" t="s">
         <v>54</v>
@@ -6449,7 +6446,7 @@
       <c r="G143" s="12"/>
       <c r="H143" s="12"/>
       <c r="I143" s="12" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="J143" s="12"/>
     </row>
@@ -6459,7 +6456,7 @@
       </c>
       <c r="B144" s="12"/>
       <c r="C144" s="16" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="D144" s="9" t="s">
         <v>54</v>
@@ -6473,55 +6470,55 @@
       <c r="G144" s="12"/>
       <c r="H144" s="12"/>
       <c r="I144" s="12" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="J144" s="12"/>
     </row>
     <row r="145" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A145" s="11" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B145" s="12"/>
       <c r="C145" s="16" t="s">
+        <v>565</v>
+      </c>
+      <c r="D145" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E145" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F145" s="13" t="s">
         <v>566</v>
-      </c>
-      <c r="D145" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E145" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="F145" s="13" t="s">
-        <v>567</v>
       </c>
       <c r="G145" s="12"/>
       <c r="H145" s="12"/>
       <c r="I145" s="12" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="J145" s="12"/>
     </row>
     <row r="146" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A146" s="11" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="B146" s="12"/>
       <c r="C146" s="16" t="s">
+        <v>568</v>
+      </c>
+      <c r="D146" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E146" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F146" s="13" t="s">
         <v>569</v>
-      </c>
-      <c r="D146" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E146" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="F146" s="13" t="s">
-        <v>570</v>
       </c>
       <c r="G146" s="12"/>
       <c r="H146" s="12"/>
       <c r="I146" s="12" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="J146" s="12"/>
     </row>
@@ -6531,7 +6528,7 @@
       </c>
       <c r="B147" s="12"/>
       <c r="C147" s="16" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="D147" s="9" t="s">
         <v>54</v>
@@ -6545,7 +6542,7 @@
       <c r="G147" s="12"/>
       <c r="H147" s="12"/>
       <c r="I147" s="12" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="J147" s="12"/>
     </row>
@@ -6555,7 +6552,7 @@
       </c>
       <c r="B148" s="12"/>
       <c r="C148" s="16" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="D148" s="9" t="s">
         <v>54</v>
@@ -6569,41 +6566,41 @@
       <c r="G148" s="12"/>
       <c r="H148" s="12"/>
       <c r="I148" s="12" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="J148" s="12"/>
     </row>
     <row r="149" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A149" s="11" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="B149" s="12"/>
       <c r="C149" s="16" t="s">
+        <v>579</v>
+      </c>
+      <c r="D149" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E149" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F149" s="13" t="s">
         <v>580</v>
-      </c>
-      <c r="D149" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E149" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="F149" s="13" t="s">
-        <v>581</v>
       </c>
       <c r="G149" s="12"/>
       <c r="H149" s="12"/>
       <c r="I149" s="12" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="J149" s="12"/>
     </row>
     <row r="150" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A150" s="17" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B150" s="12"/>
       <c r="C150" s="16" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="D150" s="9" t="s">
         <v>54</v>
@@ -6617,223 +6614,223 @@
       <c r="G150" s="12"/>
       <c r="H150" s="12"/>
       <c r="I150" s="12" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="J150" s="12"/>
     </row>
     <row r="151" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A151" s="11" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B151" s="12"/>
       <c r="C151" s="16" t="s">
+        <v>583</v>
+      </c>
+      <c r="D151" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E151" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F151" s="13" t="s">
         <v>584</v>
-      </c>
-      <c r="D151" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E151" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="F151" s="13" t="s">
-        <v>585</v>
       </c>
       <c r="G151" s="12"/>
       <c r="H151" s="12"/>
       <c r="I151" s="12" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="J151" s="12"/>
     </row>
     <row r="152" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A152" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="B152" s="12"/>
       <c r="C152" s="16" t="s">
+        <v>585</v>
+      </c>
+      <c r="D152" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E152" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F152" s="13" t="s">
         <v>586</v>
-      </c>
-      <c r="D152" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E152" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="F152" s="13" t="s">
-        <v>587</v>
       </c>
       <c r="G152" s="12"/>
       <c r="H152" s="12"/>
       <c r="I152" s="12" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="J152" s="12"/>
     </row>
     <row r="153" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A153" s="11" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="B153" s="12"/>
       <c r="C153" s="16" t="s">
+        <v>587</v>
+      </c>
+      <c r="D153" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E153" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F153" s="13" t="s">
         <v>588</v>
-      </c>
-      <c r="D153" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E153" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="F153" s="13" t="s">
-        <v>589</v>
       </c>
       <c r="G153" s="12"/>
       <c r="H153" s="12"/>
       <c r="I153" s="12" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="J153" s="12"/>
     </row>
     <row r="154" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A154" s="11" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="B154" s="12"/>
       <c r="C154" s="16" t="s">
+        <v>589</v>
+      </c>
+      <c r="D154" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E154" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F154" s="13" t="s">
         <v>590</v>
-      </c>
-      <c r="D154" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E154" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="F154" s="13" t="s">
-        <v>591</v>
       </c>
       <c r="G154" s="12"/>
       <c r="H154" s="12"/>
       <c r="I154" s="12" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="J154" s="12"/>
     </row>
     <row r="155" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A155" s="11" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="B155" s="12"/>
       <c r="C155" s="16" t="s">
+        <v>591</v>
+      </c>
+      <c r="D155" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E155" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F155" s="13" t="s">
         <v>592</v>
-      </c>
-      <c r="D155" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E155" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="F155" s="13" t="s">
-        <v>593</v>
       </c>
       <c r="G155" s="12"/>
       <c r="H155" s="12"/>
       <c r="I155" s="12" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="J155" s="12"/>
     </row>
     <row r="156" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A156" s="11" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="B156" s="12"/>
       <c r="C156" s="16" t="s">
+        <v>593</v>
+      </c>
+      <c r="D156" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E156" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F156" s="13" t="s">
         <v>594</v>
-      </c>
-      <c r="D156" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E156" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="F156" s="13" t="s">
-        <v>595</v>
       </c>
       <c r="G156" s="12"/>
       <c r="H156" s="12"/>
       <c r="I156" s="12" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="J156" s="12"/>
     </row>
     <row r="157" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A157" s="11" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B157" s="12"/>
       <c r="C157" s="16" t="s">
+        <v>595</v>
+      </c>
+      <c r="D157" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E157" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F157" s="13" t="s">
         <v>596</v>
-      </c>
-      <c r="D157" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E157" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="F157" s="13" t="s">
-        <v>597</v>
       </c>
       <c r="G157" s="12"/>
       <c r="H157" s="12"/>
       <c r="I157" s="12" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="J157" s="12"/>
     </row>
     <row r="158" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A158" s="11" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="B158" s="12"/>
       <c r="C158" s="16" t="s">
+        <v>597</v>
+      </c>
+      <c r="D158" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E158" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F158" s="13" t="s">
         <v>598</v>
-      </c>
-      <c r="D158" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E158" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="F158" s="13" t="s">
-        <v>599</v>
       </c>
       <c r="G158" s="12"/>
       <c r="H158" s="12"/>
       <c r="I158" s="12" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="J158" s="12"/>
     </row>
     <row r="159" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A159" s="11" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B159" s="12"/>
       <c r="C159" s="16" t="s">
+        <v>599</v>
+      </c>
+      <c r="D159" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E159" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F159" s="13" t="s">
         <v>600</v>
-      </c>
-      <c r="D159" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E159" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="F159" s="13" t="s">
-        <v>601</v>
       </c>
       <c r="G159" s="12"/>
       <c r="H159" s="12"/>
       <c r="I159" s="12" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="J159" s="12"/>
     </row>
@@ -6843,127 +6840,129 @@
       </c>
       <c r="B160" s="12"/>
       <c r="C160" s="16" t="s">
+        <v>601</v>
+      </c>
+      <c r="D160" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E160" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F160" s="13" t="s">
         <v>602</v>
       </c>
-      <c r="D160" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E160" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="F160" s="13" t="s">
-        <v>603</v>
-      </c>
-      <c r="G160" s="12"/>
+      <c r="G160" s="11" t="s">
+        <v>353</v>
+      </c>
       <c r="H160" s="12"/>
       <c r="I160" s="12" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="J160" s="12"/>
     </row>
     <row r="161" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A161" s="11" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B161" s="12"/>
       <c r="C161" s="16" t="s">
+        <v>603</v>
+      </c>
+      <c r="D161" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E161" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F161" s="13" t="s">
         <v>604</v>
-      </c>
-      <c r="D161" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E161" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="F161" s="13" t="s">
-        <v>605</v>
       </c>
       <c r="G161" s="12"/>
       <c r="H161" s="12"/>
       <c r="I161" s="12" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="J161" s="12"/>
     </row>
     <row r="162" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A162" s="11" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B162" s="12"/>
       <c r="C162" s="16" t="s">
+        <v>605</v>
+      </c>
+      <c r="D162" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E162" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F162" s="13" t="s">
         <v>606</v>
-      </c>
-      <c r="D162" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E162" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="F162" s="13" t="s">
-        <v>607</v>
       </c>
       <c r="G162" s="12"/>
       <c r="H162" s="12"/>
       <c r="I162" s="12" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="J162" s="12"/>
     </row>
     <row r="163" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A163" s="11" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B163" s="12"/>
       <c r="C163" s="16" t="s">
+        <v>607</v>
+      </c>
+      <c r="D163" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E163" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F163" s="13" t="s">
         <v>608</v>
-      </c>
-      <c r="D163" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E163" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="F163" s="13" t="s">
-        <v>609</v>
       </c>
       <c r="G163" s="12"/>
       <c r="H163" s="12"/>
       <c r="I163" s="12" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="J163" s="12"/>
     </row>
     <row r="164" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A164" s="11" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B164" s="12"/>
       <c r="C164" s="16" t="s">
+        <v>609</v>
+      </c>
+      <c r="D164" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E164" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F164" s="13" t="s">
         <v>610</v>
-      </c>
-      <c r="D164" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E164" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="F164" s="13" t="s">
-        <v>611</v>
       </c>
       <c r="G164" s="12"/>
       <c r="H164" s="12"/>
       <c r="I164" s="12" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="J164" s="12"/>
     </row>
     <row r="165" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A165" s="11" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="B165" s="12"/>
       <c r="C165" s="16" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="D165" s="9" t="s">
         <v>54</v>
@@ -6972,12 +6971,12 @@
         <v>108</v>
       </c>
       <c r="F165" s="13" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="G165" s="12"/>
       <c r="H165" s="12"/>
       <c r="I165" s="12" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="J165" s="12"/>
     </row>
@@ -6987,7 +6986,7 @@
       </c>
       <c r="B166" s="12"/>
       <c r="C166" s="12" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="D166" s="9" t="s">
         <v>54</v>
@@ -6996,22 +6995,22 @@
         <v>108</v>
       </c>
       <c r="F166" s="13" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="G166" s="12"/>
       <c r="H166" s="12"/>
       <c r="I166" s="12" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="J166" s="12"/>
     </row>
     <row r="167" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A167" s="11" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="B167" s="12"/>
       <c r="C167" s="16" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="D167" s="9" t="s">
         <v>54</v>
@@ -7020,22 +7019,22 @@
         <v>108</v>
       </c>
       <c r="F167" s="13" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="G167" s="12"/>
       <c r="H167" s="12"/>
       <c r="I167" s="12" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="J167" s="12"/>
     </row>
     <row r="168" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A168" s="11" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="B168" s="12"/>
       <c r="C168" s="16" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="D168" s="9" t="s">
         <v>54</v>
@@ -7044,22 +7043,22 @@
         <v>108</v>
       </c>
       <c r="F168" s="13" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="G168" s="12"/>
       <c r="H168" s="12"/>
       <c r="I168" s="12" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="J168" s="12"/>
     </row>
     <row r="169" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A169" s="11" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B169" s="12"/>
       <c r="C169" s="16" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="D169" s="9" t="s">
         <v>54</v>
@@ -7068,22 +7067,22 @@
         <v>108</v>
       </c>
       <c r="F169" s="13" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="G169" s="12"/>
       <c r="H169" s="12"/>
       <c r="I169" s="12" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="J169" s="12"/>
     </row>
     <row r="170" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A170" s="11" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="B170" s="12"/>
       <c r="C170" s="16" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="D170" s="9" t="s">
         <v>54</v>
@@ -7092,46 +7091,46 @@
         <v>108</v>
       </c>
       <c r="F170" s="13" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="G170" s="12"/>
       <c r="H170" s="12"/>
       <c r="I170" s="12" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="J170" s="12"/>
     </row>
     <row r="171" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A171" s="11" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B171" s="12"/>
       <c r="C171" s="16" t="s">
+        <v>622</v>
+      </c>
+      <c r="D171" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E171" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F171" s="13" t="s">
         <v>623</v>
-      </c>
-      <c r="D171" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E171" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="F171" s="13" t="s">
-        <v>624</v>
       </c>
       <c r="G171" s="12"/>
       <c r="H171" s="12"/>
       <c r="I171" s="12" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="J171" s="12"/>
     </row>
     <row r="172" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A172" s="11" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="B172" s="12"/>
       <c r="C172" s="16" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D172" s="9" t="s">
         <v>54</v>
@@ -7140,22 +7139,22 @@
         <v>108</v>
       </c>
       <c r="F172" s="13" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="G172" s="12"/>
       <c r="H172" s="12"/>
       <c r="I172" s="12" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="J172" s="12"/>
     </row>
     <row r="173" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A173" s="11" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B173" s="12"/>
       <c r="C173" s="16" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="D173" s="9" t="s">
         <v>54</v>
@@ -7164,60 +7163,60 @@
         <v>108</v>
       </c>
       <c r="F173" s="13" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="G173" s="12"/>
       <c r="H173" s="12"/>
       <c r="I173" s="12" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="J173" s="12"/>
     </row>
     <row r="174" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A174" s="11" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="B174" s="12"/>
       <c r="C174" s="16" t="s">
+        <v>627</v>
+      </c>
+      <c r="D174" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E174" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F174" s="13" t="s">
         <v>628</v>
-      </c>
-      <c r="D174" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E174" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="F174" s="13" t="s">
-        <v>629</v>
       </c>
       <c r="G174" s="12"/>
       <c r="H174" s="12"/>
       <c r="I174" s="12" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="J174" s="12"/>
     </row>
     <row r="175" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A175" s="11" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B175" s="12"/>
       <c r="C175" s="16" t="s">
+        <v>630</v>
+      </c>
+      <c r="D175" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E175" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F175" s="13" t="s">
         <v>631</v>
-      </c>
-      <c r="D175" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E175" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="F175" s="13" t="s">
-        <v>632</v>
       </c>
       <c r="G175" s="12"/>
       <c r="H175" s="12"/>
       <c r="I175" s="12" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="J175" s="12"/>
     </row>
@@ -7227,7 +7226,7 @@
       </c>
       <c r="B176" s="12"/>
       <c r="C176" s="16" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="D176" s="9" t="s">
         <v>54</v>
@@ -7236,22 +7235,22 @@
         <v>108</v>
       </c>
       <c r="F176" s="13" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="G176" s="12"/>
       <c r="H176" s="12"/>
       <c r="I176" s="12" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="J176" s="12"/>
     </row>
     <row r="177" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A177" s="11" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="B177" s="12"/>
       <c r="C177" s="16" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="D177" s="9" t="s">
         <v>54</v>
@@ -7260,22 +7259,22 @@
         <v>108</v>
       </c>
       <c r="F177" s="13" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="G177" s="12"/>
       <c r="H177" s="12"/>
       <c r="I177" s="12" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="J177" s="12"/>
     </row>
     <row r="178" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A178" s="17" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="B178" s="12"/>
       <c r="C178" s="16" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="D178" s="9" t="s">
         <v>54</v>
@@ -7284,22 +7283,22 @@
         <v>108</v>
       </c>
       <c r="F178" s="13" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="G178" s="12"/>
       <c r="H178" s="12"/>
       <c r="I178" s="12" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="J178" s="12"/>
     </row>
     <row r="179" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A179" s="11" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="B179" s="12"/>
       <c r="C179" s="16" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="D179" s="9" t="s">
         <v>54</v>
@@ -7308,7 +7307,7 @@
         <v>108</v>
       </c>
       <c r="F179" s="13" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="G179" s="12"/>
       <c r="H179" s="12"/>
@@ -7317,11 +7316,11 @@
     </row>
     <row r="180" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A180" s="17" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="B180" s="12"/>
       <c r="C180" s="16" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="D180" s="9" t="s">
         <v>54</v>
@@ -7330,7 +7329,7 @@
         <v>108</v>
       </c>
       <c r="F180" s="13" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="G180" s="12"/>
       <c r="H180" s="12"/>
@@ -7343,7 +7342,7 @@
       </c>
       <c r="B181" s="12"/>
       <c r="C181" s="16" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="D181" s="9" t="s">
         <v>54</v>
@@ -7361,20 +7360,20 @@
     </row>
     <row r="182" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A182" s="19" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="B182" s="20" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="C182" s="20"/>
       <c r="D182" s="21" t="s">
         <v>108</v>
       </c>
       <c r="E182" s="21" t="s">
+        <v>704</v>
+      </c>
+      <c r="F182" s="19" t="s">
         <v>705</v>
-      </c>
-      <c r="F182" s="19" t="s">
-        <v>706</v>
       </c>
       <c r="G182" s="20"/>
       <c r="H182" s="20"/>
@@ -7383,20 +7382,20 @@
     </row>
     <row r="183" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A183" s="19" t="s">
+        <v>706</v>
+      </c>
+      <c r="B183" s="20" t="s">
         <v>707</v>
-      </c>
-      <c r="B183" s="20" t="s">
-        <v>708</v>
       </c>
       <c r="C183" s="20"/>
       <c r="D183" s="21" t="s">
         <v>108</v>
       </c>
       <c r="E183" s="21" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="F183" s="19" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="G183" s="20"/>
       <c r="H183" s="20"/>
@@ -7405,17 +7404,17 @@
     </row>
     <row r="184" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A184" s="19" t="s">
+        <v>710</v>
+      </c>
+      <c r="B184" s="20" t="s">
         <v>711</v>
-      </c>
-      <c r="B184" s="20" t="s">
-        <v>712</v>
       </c>
       <c r="C184" s="20"/>
       <c r="D184" s="21" t="s">
         <v>108</v>
       </c>
       <c r="E184" s="21" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="F184" s="19" t="s">
         <v>259</v>
@@ -7427,20 +7426,20 @@
     </row>
     <row r="185" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A185" s="19" t="s">
+        <v>712</v>
+      </c>
+      <c r="B185" s="20" t="s">
         <v>713</v>
-      </c>
-      <c r="B185" s="20" t="s">
-        <v>714</v>
       </c>
       <c r="C185" s="20"/>
       <c r="D185" s="21" t="s">
         <v>108</v>
       </c>
       <c r="E185" s="21" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="F185" s="19" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="G185" s="20"/>
       <c r="H185" s="20"/>
@@ -7449,20 +7448,20 @@
     </row>
     <row r="186" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A186" s="19" t="s">
+        <v>714</v>
+      </c>
+      <c r="B186" s="20" t="s">
         <v>715</v>
-      </c>
-      <c r="B186" s="20" t="s">
-        <v>716</v>
       </c>
       <c r="C186" s="20"/>
       <c r="D186" s="21" t="s">
         <v>108</v>
       </c>
       <c r="E186" s="21" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="F186" s="19" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="G186" s="20"/>
       <c r="H186" s="20"/>
@@ -7471,20 +7470,20 @@
     </row>
     <row r="187" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A187" s="19" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="B187" s="20" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="C187" s="20"/>
       <c r="D187" s="21" t="s">
         <v>108</v>
       </c>
       <c r="E187" s="21" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="F187" s="19" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="G187" s="20"/>
       <c r="H187" s="20"/>
@@ -7493,20 +7492,20 @@
     </row>
     <row r="188" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A188" s="19" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B188" s="20" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="C188" s="20"/>
       <c r="D188" s="21" t="s">
         <v>108</v>
       </c>
       <c r="E188" s="21" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="F188" s="19" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="G188" s="20"/>
       <c r="H188" s="20"/>
@@ -7515,20 +7514,20 @@
     </row>
     <row r="189" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A189" s="19" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="B189" s="20" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="C189" s="20"/>
       <c r="D189" s="21" t="s">
         <v>108</v>
       </c>
       <c r="E189" s="21" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="F189" s="19" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="G189" s="20"/>
       <c r="H189" s="20"/>
@@ -7537,20 +7536,20 @@
     </row>
     <row r="190" spans="1:10" ht="57" x14ac:dyDescent="0.2">
       <c r="A190" s="19" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="B190" s="19" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C190" s="20"/>
       <c r="D190" s="21" t="s">
         <v>108</v>
       </c>
       <c r="E190" s="21" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="F190" s="19" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="G190" s="20"/>
       <c r="H190" s="20"/>
@@ -7559,20 +7558,20 @@
     </row>
     <row r="191" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A191" s="19" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B191" s="20" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="C191" s="20"/>
       <c r="D191" s="21" t="s">
         <v>108</v>
       </c>
       <c r="E191" s="21" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="F191" s="19" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="G191" s="20"/>
       <c r="H191" s="20"/>
@@ -7581,20 +7580,20 @@
     </row>
     <row r="192" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A192" s="19" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B192" s="20" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="C192" s="20"/>
       <c r="D192" s="21" t="s">
         <v>108</v>
       </c>
       <c r="E192" s="21" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="F192" s="19" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="G192" s="20"/>
       <c r="H192" s="20"/>

</xml_diff>

<commit_message>
See description for list of changes
REMOVED: "Register for Pickup", "Please fill in details to join this
pickup", "Register", "Name" and "Phone number"
ADDED: "You Are Not Logged-in", "If you wish register for a pickup or
to create or edit an event, please login-in." and "Login"
</commit_message>
<xml_diff>
--- a/Trans Files/Master_Translation_All_Languages.xlsx
+++ b/Trans Files/Master_Translation_All_Languages.xlsx
@@ -10,7 +10,7 @@
     <sheet name="UI_Strings" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">UI_Strings!$A$1:$H$181</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">UI_Strings!$A$1:$H$180</definedName>
   </definedNames>
   <calcPr calcId="125725" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1278" uniqueCount="744">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1281" uniqueCount="745">
   <si>
     <t>Source (English)</t>
   </si>
@@ -1715,9 +1715,6 @@
     <t>חיפוש כתובת</t>
   </si>
   <si>
-    <t>collector dialog det</t>
-  </si>
-  <si>
     <t>collector_dialog_register_text</t>
   </si>
   <si>
@@ -2138,9 +2135,6 @@
     <t>Phone</t>
   </si>
   <si>
-    <t>Login screen title</t>
-  </si>
-  <si>
     <t>???</t>
   </si>
   <si>
@@ -2260,6 +2254,15 @@
   </si>
   <si>
     <t>A small pop up information message that informs the user why we ask for his phone number</t>
+  </si>
+  <si>
+    <t>You Are Not Logged-in</t>
+  </si>
+  <si>
+    <t>If you wish register for a pickup or to create or edit an event, please login-in.</t>
+  </si>
+  <si>
+    <t>Login screen title and also an alert button title</t>
   </si>
 </sst>
 </file>
@@ -2395,15 +2398,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -2415,6 +2409,15 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -2720,10 +2723,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J192"/>
+  <dimension ref="A1:J194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B82" workbookViewId="0">
-      <selection activeCell="B88" sqref="B88"/>
+    <sheetView tabSelected="1" topLeftCell="A178" workbookViewId="0">
+      <selection activeCell="A187" sqref="A187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2774,10 +2777,10 @@
     </row>
     <row r="2" spans="1:10" ht="75" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>415</v>
@@ -2854,10 +2857,10 @@
     </row>
     <row r="5" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
+        <v>648</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>649</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>650</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="9" t="s">
@@ -3063,7 +3066,7 @@
         <v>450</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.2">
@@ -3316,7 +3319,7 @@
         <v>260</v>
       </c>
       <c r="G22" s="17" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="H22" s="12"/>
       <c r="I22" s="4" t="s">
@@ -3351,7 +3354,7 @@
         <v>452</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="30" x14ac:dyDescent="0.2">
@@ -3487,7 +3490,7 @@
         <v>453</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="30" x14ac:dyDescent="0.2">
@@ -3720,7 +3723,7 @@
         <v>306</v>
       </c>
       <c r="G37" s="17" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="H37" s="12"/>
       <c r="I37" s="4" t="s">
@@ -3858,10 +3861,10 @@
     </row>
     <row r="43" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
+        <v>650</v>
+      </c>
+      <c r="B43" s="8" t="s">
         <v>651</v>
-      </c>
-      <c r="B43" s="8" t="s">
-        <v>652</v>
       </c>
       <c r="C43" s="16" t="s">
         <v>471</v>
@@ -4107,7 +4110,7 @@
         <v>492</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>108</v>
+        <v>54</v>
       </c>
       <c r="E52" s="18" t="s">
         <v>108</v>
@@ -4589,7 +4592,7 @@
         <v>495</v>
       </c>
       <c r="D71" s="9" t="s">
-        <v>108</v>
+        <v>54</v>
       </c>
       <c r="E71" s="18" t="s">
         <v>108</v>
@@ -4718,19 +4721,21 @@
       </c>
       <c r="J75" s="4"/>
     </row>
-    <row r="76" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="8" t="s">
         <v>73</v>
       </c>
       <c r="B76" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="C76" s="4"/>
+      <c r="C76" s="16" t="s">
+        <v>563</v>
+      </c>
       <c r="D76" s="9" t="s">
-        <v>108</v>
+        <v>54</v>
       </c>
       <c r="E76" s="18" t="s">
-        <v>54</v>
+        <v>108</v>
       </c>
       <c r="F76" s="10" t="s">
         <v>264</v>
@@ -4827,7 +4832,7 @@
         <v>496</v>
       </c>
       <c r="D80" s="9" t="s">
-        <v>108</v>
+        <v>54</v>
       </c>
       <c r="E80" s="18" t="s">
         <v>108</v>
@@ -4857,7 +4862,7 @@
         <v>499</v>
       </c>
       <c r="D81" s="9" t="s">
-        <v>108</v>
+        <v>54</v>
       </c>
       <c r="E81" s="18" t="s">
         <v>108</v>
@@ -5389,7 +5394,7 @@
         <v>510</v>
       </c>
       <c r="J100" s="4" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="101" spans="1:10" ht="30" x14ac:dyDescent="0.2">
@@ -5804,10 +5809,10 @@
     </row>
     <row r="117" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A117" s="8" t="s">
+        <v>652</v>
+      </c>
+      <c r="B117" s="8" t="s">
         <v>653</v>
-      </c>
-      <c r="B117" s="8" t="s">
-        <v>654</v>
       </c>
       <c r="C117" s="4"/>
       <c r="D117" s="9" t="s">
@@ -5827,20 +5832,20 @@
       <c r="J117" s="4"/>
     </row>
     <row r="118" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A118" s="23" t="s">
-        <v>733</v>
-      </c>
-      <c r="B118" s="24"/>
-      <c r="C118" s="25" t="s">
+      <c r="A118" s="20" t="s">
+        <v>731</v>
+      </c>
+      <c r="B118" s="21"/>
+      <c r="C118" s="22" t="s">
         <v>516</v>
       </c>
-      <c r="D118" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="E118" s="26" t="s">
-        <v>108</v>
-      </c>
-      <c r="F118" s="22" t="s">
+      <c r="D118" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="E118" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="F118" s="19" t="s">
         <v>517</v>
       </c>
       <c r="G118" s="12"/>
@@ -5864,7 +5869,7 @@
       <c r="E119" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="F119" s="22" t="s">
+      <c r="F119" s="19" t="s">
         <v>223</v>
       </c>
       <c r="G119" s="12"/>
@@ -5876,7 +5881,7 @@
     </row>
     <row r="120" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A120" s="17" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="B120" s="12"/>
       <c r="C120" s="16" t="s">
@@ -5888,8 +5893,8 @@
       <c r="E120" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="F120" s="22" t="s">
-        <v>734</v>
+      <c r="F120" s="19" t="s">
+        <v>732</v>
       </c>
       <c r="G120" s="12"/>
       <c r="H120" s="12"/>
@@ -5900,7 +5905,7 @@
     </row>
     <row r="121" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A121" s="11" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="B121" s="12"/>
       <c r="C121" s="16" t="s">
@@ -5912,8 +5917,8 @@
       <c r="E121" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="F121" s="22" t="s">
-        <v>736</v>
+      <c r="F121" s="19" t="s">
+        <v>734</v>
       </c>
       <c r="G121" s="12"/>
       <c r="H121" s="12"/>
@@ -5924,7 +5929,7 @@
     </row>
     <row r="122" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A122" s="11" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="B122" s="12"/>
       <c r="C122" s="16" t="s">
@@ -5948,7 +5953,7 @@
     </row>
     <row r="123" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A123" s="17" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="B123" s="12"/>
       <c r="C123" s="16" t="s">
@@ -5960,8 +5965,8 @@
       <c r="E123" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="F123" s="22" t="s">
-        <v>737</v>
+      <c r="F123" s="19" t="s">
+        <v>735</v>
       </c>
       <c r="G123" s="12"/>
       <c r="H123" s="12"/>
@@ -5972,7 +5977,7 @@
     </row>
     <row r="124" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A124" s="11" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="B124" s="12"/>
       <c r="C124" s="16" t="s">
@@ -5996,7 +6001,7 @@
     </row>
     <row r="125" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A125" s="11" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="B125" s="12"/>
       <c r="C125" s="16" t="s">
@@ -6020,55 +6025,55 @@
     </row>
     <row r="126" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A126" s="17" t="s">
-        <v>739</v>
-      </c>
-      <c r="B126" s="24"/>
-      <c r="C126" s="25" t="s">
-        <v>571</v>
-      </c>
-      <c r="D126" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="E126" s="26" t="s">
-        <v>108</v>
-      </c>
-      <c r="F126" s="22" t="s">
-        <v>738</v>
+        <v>737</v>
+      </c>
+      <c r="B126" s="21"/>
+      <c r="C126" s="22" t="s">
+        <v>570</v>
+      </c>
+      <c r="D126" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="E126" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="F126" s="19" t="s">
+        <v>736</v>
       </c>
       <c r="G126" s="12"/>
       <c r="H126" s="12"/>
       <c r="I126" s="12" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="J126" s="12"/>
     </row>
     <row r="127" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A127" s="11" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="B127" s="12"/>
       <c r="C127" s="16" t="s">
+        <v>572</v>
+      </c>
+      <c r="D127" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E127" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F127" s="13" t="s">
         <v>573</v>
-      </c>
-      <c r="D127" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E127" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="F127" s="13" t="s">
-        <v>574</v>
       </c>
       <c r="G127" s="12"/>
       <c r="H127" s="12"/>
       <c r="I127" s="12" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="J127" s="12"/>
     </row>
     <row r="128" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A128" s="11" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="B128" s="12"/>
       <c r="C128" s="16" t="s">
@@ -6092,7 +6097,7 @@
     </row>
     <row r="129" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A129" s="11" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="B129" s="12"/>
       <c r="C129" s="16" t="s">
@@ -6116,7 +6121,7 @@
     </row>
     <row r="130" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A130" s="11" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B130" s="12"/>
       <c r="C130" s="16" t="s">
@@ -6129,7 +6134,7 @@
         <v>108</v>
       </c>
       <c r="F130" s="13" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="G130" s="12"/>
       <c r="H130" s="12"/>
@@ -6140,7 +6145,7 @@
     </row>
     <row r="131" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A131" s="11" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="B131" s="12"/>
       <c r="C131" s="16" t="s">
@@ -6164,7 +6169,7 @@
     </row>
     <row r="132" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A132" s="11" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B132" s="12"/>
       <c r="C132" s="16" t="s">
@@ -6188,7 +6193,7 @@
     </row>
     <row r="133" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A133" s="11" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="B133" s="12"/>
       <c r="C133" s="16" t="s">
@@ -6212,7 +6217,7 @@
     </row>
     <row r="134" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A134" s="11" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="B134" s="12"/>
       <c r="C134" s="16" t="s">
@@ -6236,7 +6241,7 @@
     </row>
     <row r="135" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A135" s="11" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="B135" s="12"/>
       <c r="C135" s="16" t="s">
@@ -6284,7 +6289,7 @@
     </row>
     <row r="137" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A137" s="11" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B137" s="12"/>
       <c r="C137" s="16" t="s">
@@ -6332,7 +6337,7 @@
     </row>
     <row r="139" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A139" s="11" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B139" s="12"/>
       <c r="C139" s="16" t="s">
@@ -6356,7 +6361,7 @@
     </row>
     <row r="140" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A140" s="11" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B140" s="12"/>
       <c r="C140" s="16" t="s">
@@ -6380,7 +6385,7 @@
     </row>
     <row r="141" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A141" s="11" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B141" s="12"/>
       <c r="C141" s="16" t="s">
@@ -6404,7 +6409,7 @@
     </row>
     <row r="142" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A142" s="11" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="B142" s="12"/>
       <c r="C142" s="16" t="s">
@@ -6432,7 +6437,7 @@
       </c>
       <c r="B143" s="12"/>
       <c r="C143" s="16" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="D143" s="9" t="s">
         <v>54</v>
@@ -6446,13 +6451,13 @@
       <c r="G143" s="12"/>
       <c r="H143" s="12"/>
       <c r="I143" s="12" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="J143" s="12"/>
     </row>
     <row r="144" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A144" s="11" t="s">
-        <v>73</v>
+        <v>665</v>
       </c>
       <c r="B144" s="12"/>
       <c r="C144" s="16" t="s">
@@ -6465,12 +6470,12 @@
         <v>108</v>
       </c>
       <c r="F144" s="13" t="s">
-        <v>264</v>
+        <v>565</v>
       </c>
       <c r="G144" s="12"/>
       <c r="H144" s="12"/>
       <c r="I144" s="12" t="s">
-        <v>563</v>
+        <v>566</v>
       </c>
       <c r="J144" s="12"/>
     </row>
@@ -6480,7 +6485,7 @@
       </c>
       <c r="B145" s="12"/>
       <c r="C145" s="16" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
       <c r="D145" s="9" t="s">
         <v>54</v>
@@ -6489,22 +6494,22 @@
         <v>108</v>
       </c>
       <c r="F145" s="13" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
       <c r="G145" s="12"/>
       <c r="H145" s="12"/>
       <c r="I145" s="12" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="J145" s="12"/>
     </row>
-    <row r="146" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A146" s="11" t="s">
-        <v>667</v>
+        <v>21</v>
       </c>
       <c r="B146" s="12"/>
       <c r="C146" s="16" t="s">
-        <v>568</v>
+        <v>575</v>
       </c>
       <c r="D146" s="9" t="s">
         <v>54</v>
@@ -6513,18 +6518,18 @@
         <v>108</v>
       </c>
       <c r="F146" s="13" t="s">
-        <v>569</v>
+        <v>211</v>
       </c>
       <c r="G146" s="12"/>
       <c r="H146" s="12"/>
       <c r="I146" s="12" t="s">
-        <v>567</v>
+        <v>571</v>
       </c>
       <c r="J146" s="12"/>
     </row>
     <row r="147" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A147" s="11" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B147" s="12"/>
       <c r="C147" s="16" t="s">
@@ -6537,22 +6542,22 @@
         <v>108</v>
       </c>
       <c r="F147" s="13" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="G147" s="12"/>
       <c r="H147" s="12"/>
       <c r="I147" s="12" t="s">
-        <v>572</v>
+        <v>577</v>
       </c>
       <c r="J147" s="12"/>
     </row>
     <row r="148" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A148" s="11" t="s">
-        <v>16</v>
+        <v>674</v>
       </c>
       <c r="B148" s="12"/>
       <c r="C148" s="16" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="D148" s="9" t="s">
         <v>54</v>
@@ -6561,22 +6566,22 @@
         <v>108</v>
       </c>
       <c r="F148" s="13" t="s">
-        <v>206</v>
+        <v>579</v>
       </c>
       <c r="G148" s="12"/>
       <c r="H148" s="12"/>
       <c r="I148" s="12" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
       <c r="J148" s="12"/>
     </row>
     <row r="149" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A149" s="11" t="s">
-        <v>675</v>
+      <c r="A149" s="17" t="s">
+        <v>727</v>
       </c>
       <c r="B149" s="12"/>
       <c r="C149" s="16" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
       <c r="D149" s="9" t="s">
         <v>54</v>
@@ -6584,19 +6589,19 @@
       <c r="E149" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="F149" s="13" t="s">
-        <v>580</v>
+      <c r="F149" s="19" t="s">
+        <v>267</v>
       </c>
       <c r="G149" s="12"/>
       <c r="H149" s="12"/>
       <c r="I149" s="12" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="J149" s="12"/>
     </row>
     <row r="150" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A150" s="17" t="s">
-        <v>729</v>
+      <c r="A150" s="11" t="s">
+        <v>669</v>
       </c>
       <c r="B150" s="12"/>
       <c r="C150" s="16" t="s">
@@ -6608,23 +6613,23 @@
       <c r="E150" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="F150" s="22" t="s">
-        <v>267</v>
+      <c r="F150" s="13" t="s">
+        <v>583</v>
       </c>
       <c r="G150" s="12"/>
       <c r="H150" s="12"/>
       <c r="I150" s="12" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="J150" s="12"/>
     </row>
     <row r="151" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A151" s="11" t="s">
-        <v>670</v>
+        <v>664</v>
       </c>
       <c r="B151" s="12"/>
       <c r="C151" s="16" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="D151" s="9" t="s">
         <v>54</v>
@@ -6633,22 +6638,22 @@
         <v>108</v>
       </c>
       <c r="F151" s="13" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="G151" s="12"/>
       <c r="H151" s="12"/>
       <c r="I151" s="12" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="J151" s="12"/>
     </row>
     <row r="152" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A152" s="11" t="s">
-        <v>665</v>
+        <v>675</v>
       </c>
       <c r="B152" s="12"/>
       <c r="C152" s="16" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="D152" s="9" t="s">
         <v>54</v>
@@ -6657,22 +6662,22 @@
         <v>108</v>
       </c>
       <c r="F152" s="13" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="G152" s="12"/>
       <c r="H152" s="12"/>
       <c r="I152" s="12" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="J152" s="12"/>
     </row>
-    <row r="153" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A153" s="11" t="s">
-        <v>676</v>
+        <v>667</v>
       </c>
       <c r="B153" s="12"/>
       <c r="C153" s="16" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="D153" s="9" t="s">
         <v>54</v>
@@ -6681,22 +6686,22 @@
         <v>108</v>
       </c>
       <c r="F153" s="13" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="G153" s="12"/>
       <c r="H153" s="12"/>
       <c r="I153" s="12" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="J153" s="12"/>
     </row>
-    <row r="154" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A154" s="11" t="s">
         <v>668</v>
       </c>
       <c r="B154" s="12"/>
       <c r="C154" s="16" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="D154" s="9" t="s">
         <v>54</v>
@@ -6705,22 +6710,22 @@
         <v>108</v>
       </c>
       <c r="F154" s="13" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="G154" s="12"/>
       <c r="H154" s="12"/>
       <c r="I154" s="12" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="J154" s="12"/>
     </row>
     <row r="155" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A155" s="11" t="s">
-        <v>669</v>
+        <v>676</v>
       </c>
       <c r="B155" s="12"/>
       <c r="C155" s="16" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="D155" s="9" t="s">
         <v>54</v>
@@ -6729,22 +6734,22 @@
         <v>108</v>
       </c>
       <c r="F155" s="13" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="G155" s="12"/>
       <c r="H155" s="12"/>
       <c r="I155" s="12" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="J155" s="12"/>
     </row>
     <row r="156" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A156" s="11" t="s">
-        <v>677</v>
+        <v>663</v>
       </c>
       <c r="B156" s="12"/>
       <c r="C156" s="16" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="D156" s="9" t="s">
         <v>54</v>
@@ -6753,22 +6758,22 @@
         <v>108</v>
       </c>
       <c r="F156" s="13" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="G156" s="12"/>
       <c r="H156" s="12"/>
       <c r="I156" s="12" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="J156" s="12"/>
     </row>
     <row r="157" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A157" s="11" t="s">
-        <v>664</v>
+        <v>670</v>
       </c>
       <c r="B157" s="12"/>
       <c r="C157" s="16" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="D157" s="9" t="s">
         <v>54</v>
@@ -6777,12 +6782,12 @@
         <v>108</v>
       </c>
       <c r="F157" s="13" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="G157" s="12"/>
       <c r="H157" s="12"/>
       <c r="I157" s="12" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="J157" s="12"/>
     </row>
@@ -6792,7 +6797,7 @@
       </c>
       <c r="B158" s="12"/>
       <c r="C158" s="16" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="D158" s="9" t="s">
         <v>54</v>
@@ -6801,22 +6806,22 @@
         <v>108</v>
       </c>
       <c r="F158" s="13" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="G158" s="12"/>
       <c r="H158" s="12"/>
       <c r="I158" s="12" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="J158" s="12"/>
     </row>
     <row r="159" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A159" s="11" t="s">
-        <v>672</v>
+        <v>51</v>
       </c>
       <c r="B159" s="12"/>
       <c r="C159" s="16" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="D159" s="9" t="s">
         <v>54</v>
@@ -6825,22 +6830,24 @@
         <v>108</v>
       </c>
       <c r="F159" s="13" t="s">
-        <v>600</v>
-      </c>
-      <c r="G159" s="12"/>
+        <v>601</v>
+      </c>
+      <c r="G159" s="11" t="s">
+        <v>353</v>
+      </c>
       <c r="H159" s="12"/>
       <c r="I159" s="12" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="J159" s="12"/>
     </row>
     <row r="160" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A160" s="11" t="s">
-        <v>51</v>
+        <v>672</v>
       </c>
       <c r="B160" s="12"/>
       <c r="C160" s="16" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="D160" s="9" t="s">
         <v>54</v>
@@ -6849,24 +6856,22 @@
         <v>108</v>
       </c>
       <c r="F160" s="13" t="s">
-        <v>602</v>
-      </c>
-      <c r="G160" s="11" t="s">
-        <v>353</v>
-      </c>
+        <v>603</v>
+      </c>
+      <c r="G160" s="12"/>
       <c r="H160" s="12"/>
       <c r="I160" s="12" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="J160" s="12"/>
     </row>
     <row r="161" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A161" s="11" t="s">
-        <v>673</v>
+        <v>677</v>
       </c>
       <c r="B161" s="12"/>
       <c r="C161" s="16" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="D161" s="9" t="s">
         <v>54</v>
@@ -6875,12 +6880,12 @@
         <v>108</v>
       </c>
       <c r="F161" s="13" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="G161" s="12"/>
       <c r="H161" s="12"/>
       <c r="I161" s="12" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="J161" s="12"/>
     </row>
@@ -6890,7 +6895,7 @@
       </c>
       <c r="B162" s="12"/>
       <c r="C162" s="16" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="D162" s="9" t="s">
         <v>54</v>
@@ -6899,12 +6904,12 @@
         <v>108</v>
       </c>
       <c r="F162" s="13" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="G162" s="12"/>
       <c r="H162" s="12"/>
       <c r="I162" s="12" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="J162" s="12"/>
     </row>
@@ -6914,7 +6919,7 @@
       </c>
       <c r="B163" s="12"/>
       <c r="C163" s="16" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="D163" s="9" t="s">
         <v>54</v>
@@ -6923,22 +6928,22 @@
         <v>108</v>
       </c>
       <c r="F163" s="13" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="G163" s="12"/>
       <c r="H163" s="12"/>
       <c r="I163" s="12" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="J163" s="12"/>
     </row>
     <row r="164" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A164" s="11" t="s">
-        <v>680</v>
+        <v>683</v>
       </c>
       <c r="B164" s="12"/>
       <c r="C164" s="16" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="D164" s="9" t="s">
         <v>54</v>
@@ -6947,21 +6952,21 @@
         <v>108</v>
       </c>
       <c r="F164" s="13" t="s">
-        <v>610</v>
+        <v>612</v>
       </c>
       <c r="G164" s="12"/>
       <c r="H164" s="12"/>
       <c r="I164" s="12" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="J164" s="12"/>
     </row>
-    <row r="165" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A165" s="11" t="s">
-        <v>684</v>
+        <v>42</v>
       </c>
       <c r="B165" s="12"/>
-      <c r="C165" s="16" t="s">
+      <c r="C165" s="12" t="s">
         <v>611</v>
       </c>
       <c r="D165" s="9" t="s">
@@ -6976,17 +6981,17 @@
       <c r="G165" s="12"/>
       <c r="H165" s="12"/>
       <c r="I165" s="12" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="J165" s="12"/>
     </row>
-    <row r="166" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A166" s="11" t="s">
-        <v>42</v>
+        <v>684</v>
       </c>
       <c r="B166" s="12"/>
-      <c r="C166" s="12" t="s">
-        <v>612</v>
+      <c r="C166" s="16" t="s">
+        <v>614</v>
       </c>
       <c r="D166" s="9" t="s">
         <v>54</v>
@@ -6995,16 +7000,16 @@
         <v>108</v>
       </c>
       <c r="F166" s="13" t="s">
-        <v>614</v>
+        <v>552</v>
       </c>
       <c r="G166" s="12"/>
       <c r="H166" s="12"/>
       <c r="I166" s="12" t="s">
-        <v>581</v>
+        <v>481</v>
       </c>
       <c r="J166" s="12"/>
     </row>
-    <row r="167" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A167" s="11" t="s">
         <v>685</v>
       </c>
@@ -7019,7 +7024,7 @@
         <v>108</v>
       </c>
       <c r="F167" s="13" t="s">
-        <v>552</v>
+        <v>618</v>
       </c>
       <c r="G167" s="12"/>
       <c r="H167" s="12"/>
@@ -7028,7 +7033,7 @@
       </c>
       <c r="J167" s="12"/>
     </row>
-    <row r="168" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A168" s="11" t="s">
         <v>686</v>
       </c>
@@ -7052,7 +7057,7 @@
       </c>
       <c r="J168" s="12"/>
     </row>
-    <row r="169" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A169" s="11" t="s">
         <v>687</v>
       </c>
@@ -7076,13 +7081,13 @@
       </c>
       <c r="J169" s="12"/>
     </row>
-    <row r="170" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A170" s="11" t="s">
         <v>688</v>
       </c>
       <c r="B170" s="12"/>
       <c r="C170" s="16" t="s">
-        <v>618</v>
+        <v>621</v>
       </c>
       <c r="D170" s="9" t="s">
         <v>54</v>
@@ -7091,22 +7096,22 @@
         <v>108</v>
       </c>
       <c r="F170" s="13" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="G170" s="12"/>
       <c r="H170" s="12"/>
       <c r="I170" s="12" t="s">
-        <v>481</v>
+        <v>624</v>
       </c>
       <c r="J170" s="12"/>
     </row>
-    <row r="171" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A171" s="11" t="s">
         <v>689</v>
       </c>
       <c r="B171" s="12"/>
       <c r="C171" s="16" t="s">
-        <v>622</v>
+        <v>423</v>
       </c>
       <c r="D171" s="9" t="s">
         <v>54</v>
@@ -7120,17 +7125,17 @@
       <c r="G171" s="12"/>
       <c r="H171" s="12"/>
       <c r="I171" s="12" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="J171" s="12"/>
     </row>
-    <row r="172" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A172" s="11" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="B172" s="12"/>
       <c r="C172" s="16" t="s">
-        <v>423</v>
+        <v>625</v>
       </c>
       <c r="D172" s="9" t="s">
         <v>54</v>
@@ -7139,18 +7144,18 @@
         <v>108</v>
       </c>
       <c r="F172" s="13" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="G172" s="12"/>
       <c r="H172" s="12"/>
       <c r="I172" s="12" t="s">
-        <v>625</v>
+        <v>628</v>
       </c>
       <c r="J172" s="12"/>
     </row>
     <row r="173" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A173" s="11" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="B173" s="12"/>
       <c r="C173" s="16" t="s">
@@ -7163,22 +7168,22 @@
         <v>108</v>
       </c>
       <c r="F173" s="13" t="s">
-        <v>623</v>
+        <v>627</v>
       </c>
       <c r="G173" s="12"/>
       <c r="H173" s="12"/>
       <c r="I173" s="12" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="J173" s="12"/>
     </row>
     <row r="174" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A174" s="11" t="s">
-        <v>691</v>
+        <v>700</v>
       </c>
       <c r="B174" s="12"/>
       <c r="C174" s="16" t="s">
-        <v>627</v>
+        <v>629</v>
       </c>
       <c r="D174" s="9" t="s">
         <v>54</v>
@@ -7187,22 +7192,22 @@
         <v>108</v>
       </c>
       <c r="F174" s="13" t="s">
-        <v>628</v>
+        <v>630</v>
       </c>
       <c r="G174" s="12"/>
       <c r="H174" s="12"/>
       <c r="I174" s="12" t="s">
-        <v>629</v>
+        <v>631</v>
       </c>
       <c r="J174" s="12"/>
     </row>
     <row r="175" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A175" s="11" t="s">
-        <v>701</v>
+        <v>52</v>
       </c>
       <c r="B175" s="12"/>
       <c r="C175" s="16" t="s">
-        <v>630</v>
+        <v>632</v>
       </c>
       <c r="D175" s="9" t="s">
         <v>54</v>
@@ -7211,18 +7216,18 @@
         <v>108</v>
       </c>
       <c r="F175" s="13" t="s">
-        <v>631</v>
+        <v>637</v>
       </c>
       <c r="G175" s="12"/>
       <c r="H175" s="12"/>
       <c r="I175" s="12" t="s">
-        <v>632</v>
+        <v>638</v>
       </c>
       <c r="J175" s="12"/>
     </row>
     <row r="176" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A176" s="11" t="s">
-        <v>52</v>
+        <v>691</v>
       </c>
       <c r="B176" s="12"/>
       <c r="C176" s="16" t="s">
@@ -7235,18 +7240,18 @@
         <v>108</v>
       </c>
       <c r="F176" s="13" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="G176" s="12"/>
       <c r="H176" s="12"/>
       <c r="I176" s="12" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="J176" s="12"/>
     </row>
     <row r="177" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A177" s="11" t="s">
-        <v>692</v>
+      <c r="A177" s="17" t="s">
+        <v>738</v>
       </c>
       <c r="B177" s="12"/>
       <c r="C177" s="16" t="s">
@@ -7264,17 +7269,17 @@
       <c r="G177" s="12"/>
       <c r="H177" s="12"/>
       <c r="I177" s="12" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="J177" s="12"/>
     </row>
     <row r="178" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A178" s="17" t="s">
-        <v>740</v>
+      <c r="A178" s="11" t="s">
+        <v>692</v>
       </c>
       <c r="B178" s="12"/>
       <c r="C178" s="16" t="s">
-        <v>635</v>
+        <v>639</v>
       </c>
       <c r="D178" s="9" t="s">
         <v>54</v>
@@ -7283,18 +7288,16 @@
         <v>108</v>
       </c>
       <c r="F178" s="13" t="s">
-        <v>637</v>
+        <v>642</v>
       </c>
       <c r="G178" s="12"/>
       <c r="H178" s="12"/>
-      <c r="I178" s="12" t="s">
-        <v>639</v>
-      </c>
+      <c r="I178" s="12"/>
       <c r="J178" s="12"/>
     </row>
     <row r="179" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A179" s="11" t="s">
-        <v>693</v>
+      <c r="A179" s="17" t="s">
+        <v>740</v>
       </c>
       <c r="B179" s="12"/>
       <c r="C179" s="16" t="s">
@@ -7307,7 +7310,7 @@
         <v>108</v>
       </c>
       <c r="F179" s="13" t="s">
-        <v>643</v>
+        <v>739</v>
       </c>
       <c r="G179" s="12"/>
       <c r="H179" s="12"/>
@@ -7316,292 +7319,322 @@
     </row>
     <row r="180" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A180" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B180" s="21"/>
+      <c r="C180" s="22" t="s">
+        <v>641</v>
+      </c>
+      <c r="D180" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="E180" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="F180" s="19" t="s">
+        <v>211</v>
+      </c>
+      <c r="G180" s="21"/>
+      <c r="H180" s="21"/>
+      <c r="I180" s="21"/>
+      <c r="J180" s="21"/>
+    </row>
+    <row r="181" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A181" s="24" t="s">
+        <v>701</v>
+      </c>
+      <c r="B181" s="25" t="s">
+        <v>707</v>
+      </c>
+      <c r="C181" s="25"/>
+      <c r="D181" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="E181" s="26" t="s">
+        <v>702</v>
+      </c>
+      <c r="F181" s="24" t="s">
+        <v>703</v>
+      </c>
+      <c r="G181" s="25"/>
+      <c r="H181" s="25"/>
+      <c r="I181" s="25"/>
+      <c r="J181" s="25"/>
+    </row>
+    <row r="182" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A182" s="24" t="s">
+        <v>704</v>
+      </c>
+      <c r="B182" s="25" t="s">
+        <v>705</v>
+      </c>
+      <c r="C182" s="25"/>
+      <c r="D182" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="E182" s="26" t="s">
+        <v>702</v>
+      </c>
+      <c r="F182" s="24" t="s">
+        <v>706</v>
+      </c>
+      <c r="G182" s="25"/>
+      <c r="H182" s="25"/>
+      <c r="I182" s="25"/>
+      <c r="J182" s="25"/>
+    </row>
+    <row r="183" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A183" s="24" t="s">
+        <v>708</v>
+      </c>
+      <c r="B183" s="25" t="s">
+        <v>709</v>
+      </c>
+      <c r="C183" s="25"/>
+      <c r="D183" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="E183" s="26" t="s">
+        <v>702</v>
+      </c>
+      <c r="F183" s="24" t="s">
+        <v>259</v>
+      </c>
+      <c r="G183" s="25"/>
+      <c r="H183" s="25"/>
+      <c r="I183" s="25"/>
+      <c r="J183" s="25"/>
+    </row>
+    <row r="184" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A184" s="24" t="s">
+        <v>710</v>
+      </c>
+      <c r="B184" s="25" t="s">
+        <v>711</v>
+      </c>
+      <c r="C184" s="25"/>
+      <c r="D184" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="E184" s="26" t="s">
+        <v>702</v>
+      </c>
+      <c r="F184" s="24" t="s">
+        <v>710</v>
+      </c>
+      <c r="G184" s="25"/>
+      <c r="H184" s="25"/>
+      <c r="I184" s="25"/>
+      <c r="J184" s="25"/>
+    </row>
+    <row r="185" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A185" s="24" t="s">
+        <v>712</v>
+      </c>
+      <c r="B185" s="25" t="s">
+        <v>713</v>
+      </c>
+      <c r="C185" s="25"/>
+      <c r="D185" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="E185" s="26" t="s">
+        <v>702</v>
+      </c>
+      <c r="F185" s="24" t="s">
+        <v>714</v>
+      </c>
+      <c r="G185" s="25"/>
+      <c r="H185" s="25"/>
+      <c r="I185" s="25"/>
+      <c r="J185" s="25"/>
+    </row>
+    <row r="186" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A186" s="24" t="s">
+        <v>715</v>
+      </c>
+      <c r="B186" s="25" t="s">
+        <v>713</v>
+      </c>
+      <c r="C186" s="25"/>
+      <c r="D186" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="E186" s="26" t="s">
+        <v>702</v>
+      </c>
+      <c r="F186" s="24" t="s">
+        <v>716</v>
+      </c>
+      <c r="G186" s="25"/>
+      <c r="H186" s="25"/>
+      <c r="I186" s="25"/>
+      <c r="J186" s="25"/>
+    </row>
+    <row r="187" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A187" s="24" t="s">
+        <v>717</v>
+      </c>
+      <c r="B187" s="25" t="s">
+        <v>705</v>
+      </c>
+      <c r="C187" s="25"/>
+      <c r="D187" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="E187" s="26" t="s">
+        <v>702</v>
+      </c>
+      <c r="F187" s="24" t="s">
+        <v>718</v>
+      </c>
+      <c r="G187" s="25"/>
+      <c r="H187" s="25"/>
+      <c r="I187" s="25"/>
+      <c r="J187" s="25"/>
+    </row>
+    <row r="188" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A188" s="24" t="s">
+        <v>719</v>
+      </c>
+      <c r="B188" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="C188" s="25"/>
+      <c r="D188" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="E188" s="26" t="s">
+        <v>702</v>
+      </c>
+      <c r="F188" s="24" t="s">
+        <v>720</v>
+      </c>
+      <c r="G188" s="25"/>
+      <c r="H188" s="25"/>
+      <c r="I188" s="25"/>
+      <c r="J188" s="25"/>
+    </row>
+    <row r="189" spans="1:10" ht="57" x14ac:dyDescent="0.2">
+      <c r="A189" s="24" t="s">
+        <v>721</v>
+      </c>
+      <c r="B189" s="24" t="s">
+        <v>741</v>
+      </c>
+      <c r="C189" s="25"/>
+      <c r="D189" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="E189" s="26" t="s">
+        <v>702</v>
+      </c>
+      <c r="F189" s="24" t="s">
+        <v>722</v>
+      </c>
+      <c r="G189" s="25"/>
+      <c r="H189" s="25"/>
+      <c r="I189" s="25"/>
+      <c r="J189" s="25"/>
+    </row>
+    <row r="190" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A190" s="24" t="s">
+        <v>723</v>
+      </c>
+      <c r="B190" s="25" t="s">
+        <v>725</v>
+      </c>
+      <c r="C190" s="25"/>
+      <c r="D190" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="E190" s="26" t="s">
+        <v>702</v>
+      </c>
+      <c r="F190" s="24" t="s">
+        <v>724</v>
+      </c>
+      <c r="G190" s="25"/>
+      <c r="H190" s="25"/>
+      <c r="I190" s="25"/>
+      <c r="J190" s="25"/>
+    </row>
+    <row r="191" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A191" s="24" t="s">
+        <v>728</v>
+      </c>
+      <c r="B191" s="25" t="s">
+        <v>725</v>
+      </c>
+      <c r="C191" s="25"/>
+      <c r="D191" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="E191" s="26" t="s">
+        <v>702</v>
+      </c>
+      <c r="F191" s="24" t="s">
+        <v>729</v>
+      </c>
+      <c r="G191" s="25"/>
+      <c r="H191" s="25"/>
+      <c r="I191" s="25"/>
+      <c r="J191" s="25"/>
+    </row>
+    <row r="192" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A192" s="24" t="s">
         <v>742</v>
       </c>
-      <c r="B180" s="12"/>
-      <c r="C180" s="16" t="s">
-        <v>641</v>
-      </c>
-      <c r="D180" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E180" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="F180" s="13" t="s">
-        <v>741</v>
-      </c>
-      <c r="G180" s="12"/>
-      <c r="H180" s="12"/>
-      <c r="I180" s="12"/>
-      <c r="J180" s="12"/>
-    </row>
-    <row r="181" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A181" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B181" s="12"/>
-      <c r="C181" s="16" t="s">
-        <v>642</v>
-      </c>
-      <c r="D181" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E181" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="F181" s="13" t="s">
-        <v>211</v>
-      </c>
-      <c r="G181" s="12"/>
-      <c r="H181" s="12"/>
-      <c r="I181" s="12"/>
-      <c r="J181" s="12"/>
-    </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A182" s="19" t="s">
+      <c r="B192" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="C192" s="25"/>
+      <c r="D192" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="E192" s="26" t="s">
         <v>702</v>
       </c>
-      <c r="B182" s="20" t="s">
-        <v>709</v>
-      </c>
-      <c r="C182" s="20"/>
-      <c r="D182" s="21" t="s">
-        <v>108</v>
-      </c>
-      <c r="E182" s="21" t="s">
-        <v>704</v>
-      </c>
-      <c r="F182" s="19" t="s">
-        <v>705</v>
-      </c>
-      <c r="G182" s="20"/>
-      <c r="H182" s="20"/>
-      <c r="I182" s="20"/>
-      <c r="J182" s="20"/>
-    </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A183" s="19" t="s">
-        <v>706</v>
-      </c>
-      <c r="B183" s="20" t="s">
-        <v>707</v>
-      </c>
-      <c r="C183" s="20"/>
-      <c r="D183" s="21" t="s">
-        <v>108</v>
-      </c>
-      <c r="E183" s="21" t="s">
-        <v>704</v>
-      </c>
-      <c r="F183" s="19" t="s">
-        <v>708</v>
-      </c>
-      <c r="G183" s="20"/>
-      <c r="H183" s="20"/>
-      <c r="I183" s="20"/>
-      <c r="J183" s="20"/>
-    </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A184" s="19" t="s">
-        <v>710</v>
-      </c>
-      <c r="B184" s="20" t="s">
-        <v>711</v>
-      </c>
-      <c r="C184" s="20"/>
-      <c r="D184" s="21" t="s">
-        <v>108</v>
-      </c>
-      <c r="E184" s="21" t="s">
-        <v>704</v>
-      </c>
-      <c r="F184" s="19" t="s">
-        <v>259</v>
-      </c>
-      <c r="G184" s="20"/>
-      <c r="H184" s="20"/>
-      <c r="I184" s="20"/>
-      <c r="J184" s="20"/>
-    </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A185" s="19" t="s">
-        <v>712</v>
-      </c>
-      <c r="B185" s="20" t="s">
-        <v>713</v>
-      </c>
-      <c r="C185" s="20"/>
-      <c r="D185" s="21" t="s">
-        <v>108</v>
-      </c>
-      <c r="E185" s="21" t="s">
-        <v>704</v>
-      </c>
-      <c r="F185" s="19" t="s">
-        <v>712</v>
-      </c>
-      <c r="G185" s="20"/>
-      <c r="H185" s="20"/>
-      <c r="I185" s="20"/>
-      <c r="J185" s="20"/>
-    </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A186" s="19" t="s">
-        <v>714</v>
-      </c>
-      <c r="B186" s="20" t="s">
-        <v>715</v>
-      </c>
-      <c r="C186" s="20"/>
-      <c r="D186" s="21" t="s">
-        <v>108</v>
-      </c>
-      <c r="E186" s="21" t="s">
-        <v>704</v>
-      </c>
-      <c r="F186" s="19" t="s">
-        <v>716</v>
-      </c>
-      <c r="G186" s="20"/>
-      <c r="H186" s="20"/>
-      <c r="I186" s="20"/>
-      <c r="J186" s="20"/>
-    </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A187" s="19" t="s">
-        <v>717</v>
-      </c>
-      <c r="B187" s="20" t="s">
-        <v>715</v>
-      </c>
-      <c r="C187" s="20"/>
-      <c r="D187" s="21" t="s">
-        <v>108</v>
-      </c>
-      <c r="E187" s="21" t="s">
-        <v>704</v>
-      </c>
-      <c r="F187" s="19" t="s">
-        <v>718</v>
-      </c>
-      <c r="G187" s="20"/>
-      <c r="H187" s="20"/>
-      <c r="I187" s="20"/>
-      <c r="J187" s="20"/>
-    </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A188" s="19" t="s">
-        <v>719</v>
-      </c>
-      <c r="B188" s="20" t="s">
-        <v>707</v>
-      </c>
-      <c r="C188" s="20"/>
-      <c r="D188" s="21" t="s">
-        <v>108</v>
-      </c>
-      <c r="E188" s="21" t="s">
-        <v>704</v>
-      </c>
-      <c r="F188" s="19" t="s">
-        <v>720</v>
-      </c>
-      <c r="G188" s="20"/>
-      <c r="H188" s="20"/>
-      <c r="I188" s="20"/>
-      <c r="J188" s="20"/>
-    </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A189" s="19" t="s">
-        <v>721</v>
-      </c>
-      <c r="B189" s="20" t="s">
-        <v>703</v>
-      </c>
-      <c r="C189" s="20"/>
-      <c r="D189" s="21" t="s">
-        <v>108</v>
-      </c>
-      <c r="E189" s="21" t="s">
-        <v>704</v>
-      </c>
-      <c r="F189" s="19" t="s">
-        <v>722</v>
-      </c>
-      <c r="G189" s="20"/>
-      <c r="H189" s="20"/>
-      <c r="I189" s="20"/>
-      <c r="J189" s="20"/>
-    </row>
-    <row r="190" spans="1:10" ht="57" x14ac:dyDescent="0.2">
-      <c r="A190" s="19" t="s">
-        <v>723</v>
-      </c>
-      <c r="B190" s="19" t="s">
+      <c r="F192" s="24"/>
+      <c r="G192" s="25"/>
+      <c r="H192" s="25"/>
+      <c r="I192" s="25"/>
+      <c r="J192" s="25"/>
+    </row>
+    <row r="193" spans="1:10" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A193" s="24" t="s">
         <v>743</v>
       </c>
-      <c r="C190" s="20"/>
-      <c r="D190" s="21" t="s">
-        <v>108</v>
-      </c>
-      <c r="E190" s="21" t="s">
-        <v>704</v>
-      </c>
-      <c r="F190" s="19" t="s">
-        <v>724</v>
-      </c>
-      <c r="G190" s="20"/>
-      <c r="H190" s="20"/>
-      <c r="I190" s="20"/>
-      <c r="J190" s="20"/>
-    </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A191" s="19" t="s">
-        <v>725</v>
-      </c>
-      <c r="B191" s="20" t="s">
-        <v>727</v>
-      </c>
-      <c r="C191" s="20"/>
-      <c r="D191" s="21" t="s">
-        <v>108</v>
-      </c>
-      <c r="E191" s="21" t="s">
-        <v>704</v>
-      </c>
-      <c r="F191" s="19" t="s">
-        <v>726</v>
-      </c>
-      <c r="G191" s="20"/>
-      <c r="H191" s="20"/>
-      <c r="I191" s="20"/>
-      <c r="J191" s="20"/>
-    </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A192" s="19" t="s">
-        <v>730</v>
-      </c>
-      <c r="B192" s="20" t="s">
-        <v>727</v>
-      </c>
-      <c r="C192" s="20"/>
-      <c r="D192" s="21" t="s">
-        <v>108</v>
-      </c>
-      <c r="E192" s="21" t="s">
-        <v>704</v>
-      </c>
-      <c r="F192" s="19" t="s">
-        <v>731</v>
-      </c>
-      <c r="G192" s="20"/>
-      <c r="H192" s="20"/>
-      <c r="I192" s="20"/>
-      <c r="J192" s="20"/>
+      <c r="B193" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="C193" s="25"/>
+      <c r="D193" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="E193" s="26" t="s">
+        <v>702</v>
+      </c>
+      <c r="F193" s="24"/>
+      <c r="G193" s="25"/>
+      <c r="H193" s="25"/>
+      <c r="I193" s="25"/>
+      <c r="J193" s="25"/>
+    </row>
+    <row r="194" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A194" s="24"/>
+      <c r="B194" s="25"/>
+      <c r="C194" s="25"/>
+      <c r="D194" s="26"/>
+      <c r="E194" s="26"/>
+      <c r="F194" s="24"/>
+      <c r="G194" s="25"/>
+      <c r="H194" s="25"/>
+      <c r="I194" s="25"/>
+      <c r="J194" s="25"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H181"/>
+  <autoFilter ref="A1:H180"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>